<commit_message>
Added Biological Age based off of % Adult Height
</commit_message>
<xml_diff>
--- a/data-raw/maturation.xlsx
+++ b/data-raw/maturation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdukikhia/Documents/R Packages/ageR/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00256E14-F28F-6F4F-8AD6-A5F6DE9EEE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04F370-A91D-F642-A7A7-E5200F86C3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17640" xr2:uid="{1F346313-5E37-0D4E-9152-608513635295}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17640" activeTab="5" xr2:uid="{1F346313-5E37-0D4E-9152-608513635295}"/>
   </bookViews>
   <sheets>
     <sheet name="maturation" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="CDC curves" sheetId="3" r:id="rId3"/>
     <sheet name="UK90 curves" sheetId="4" r:id="rId4"/>
     <sheet name="Zscores" sheetId="5" r:id="rId5"/>
+    <sheet name="Bio Age" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="75">
   <si>
     <t>Player Name</t>
   </si>
@@ -253,6 +254,18 @@
   </si>
   <si>
     <t>U13</t>
+  </si>
+  <si>
+    <t>%PAH</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Height (cm)</t>
+  </si>
+  <si>
+    <t>Biological Age</t>
   </si>
 </sst>
 </file>
@@ -629,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530614B8-B2C3-9642-8C2E-3CA3DEE7E5A6}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -31106,4 +31119,3071 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4643ECC-1455-254C-B38F-4BE8DEA7347B}">
+  <dimension ref="A1:D218"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>28.746832000000001</v>
+      </c>
+      <c r="B2">
+        <v>30.808223000000002</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>51.04</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>30.808223000000002</v>
+      </c>
+      <c r="B3">
+        <v>32.717543999999997</v>
+      </c>
+      <c r="C3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="D3">
+        <v>54.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>32.717543999999997</v>
+      </c>
+      <c r="B4">
+        <v>34.395944999999998</v>
+      </c>
+      <c r="C4">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D4">
+        <v>58.09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>34.395944999999998</v>
+      </c>
+      <c r="B5">
+        <v>35.815263000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+      <c r="D5">
+        <v>61.07</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>35.815263000000002</v>
+      </c>
+      <c r="B6">
+        <v>37.009293</v>
+      </c>
+      <c r="C6">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="D6">
+        <v>63.59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>37.009293</v>
+      </c>
+      <c r="B7">
+        <v>38.011828000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="D7">
+        <v>65.709999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>38.011828000000001</v>
+      </c>
+      <c r="B8">
+        <v>38.884821000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
+        <v>67.489999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>38.884821000000002</v>
+      </c>
+      <c r="B9">
+        <v>39.678964000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="D9">
+        <v>69.040000000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>39.678964000000001</v>
+      </c>
+      <c r="B10">
+        <v>40.428047999999997</v>
+      </c>
+      <c r="C10">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="D10">
+        <v>70.45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>40.428047999999997</v>
+      </c>
+      <c r="B11">
+        <v>41.154603999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.75</v>
+      </c>
+      <c r="D11">
+        <v>71.78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>41.154603999999999</v>
+      </c>
+      <c r="B12">
+        <v>41.858631000000003</v>
+      </c>
+      <c r="C12">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="D12">
+        <v>73.069999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>41.858631000000003</v>
+      </c>
+      <c r="B13">
+        <v>42.528865000000003</v>
+      </c>
+      <c r="C13">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="D13">
+        <v>74.319999999999993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>42.528865000000003</v>
+      </c>
+      <c r="B14">
+        <v>43.170938</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>75.510000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>43.170938</v>
+      </c>
+      <c r="B15">
+        <v>43.784849000000001</v>
+      </c>
+      <c r="C15">
+        <v>1.083</v>
+      </c>
+      <c r="D15">
+        <v>76.650000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>43.784849000000001</v>
+      </c>
+      <c r="B16">
+        <v>44.376232000000002</v>
+      </c>
+      <c r="C16">
+        <v>1.167</v>
+      </c>
+      <c r="D16">
+        <v>77.739999999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>44.376232000000002</v>
+      </c>
+      <c r="B17">
+        <v>44.950718000000002</v>
+      </c>
+      <c r="C17">
+        <v>1.25</v>
+      </c>
+      <c r="D17">
+        <v>78.790000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>44.950718000000002</v>
+      </c>
+      <c r="B18">
+        <v>45.502675000000004</v>
+      </c>
+      <c r="C18">
+        <v>1.333</v>
+      </c>
+      <c r="D18">
+        <v>79.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>45.502675000000004</v>
+      </c>
+      <c r="B19">
+        <v>46.037736000000002</v>
+      </c>
+      <c r="C19">
+        <v>1.417</v>
+      </c>
+      <c r="D19">
+        <v>80.790000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>46.037736000000002</v>
+      </c>
+      <c r="B20">
+        <v>46.555900000000001</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+      <c r="D20">
+        <v>81.739999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>46.555900000000001</v>
+      </c>
+      <c r="B21">
+        <v>47.051535000000001</v>
+      </c>
+      <c r="C21">
+        <v>1.583</v>
+      </c>
+      <c r="D21">
+        <v>82.66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>47.051535000000001</v>
+      </c>
+      <c r="B22">
+        <v>47.535905</v>
+      </c>
+      <c r="C22">
+        <v>1.667</v>
+      </c>
+      <c r="D22">
+        <v>83.54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>47.535905</v>
+      </c>
+      <c r="B23">
+        <v>47.997746999999997</v>
+      </c>
+      <c r="C23">
+        <v>1.75</v>
+      </c>
+      <c r="D23">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>47.997746999999997</v>
+      </c>
+      <c r="B24">
+        <v>48.448324</v>
+      </c>
+      <c r="C24">
+        <v>1.833</v>
+      </c>
+      <c r="D24">
+        <v>85.22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>48.448324</v>
+      </c>
+      <c r="B25">
+        <v>48.887636999999998</v>
+      </c>
+      <c r="C25">
+        <v>1.917</v>
+      </c>
+      <c r="D25">
+        <v>86.02</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>48.887636999999998</v>
+      </c>
+      <c r="B26">
+        <v>49.315685999999999</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>49.315685999999999</v>
+      </c>
+      <c r="B27">
+        <v>49.738101999999998</v>
+      </c>
+      <c r="C27">
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="D27">
+        <v>87.56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>49.738101999999998</v>
+      </c>
+      <c r="B28">
+        <v>50.149253999999999</v>
+      </c>
+      <c r="C28">
+        <v>2.1669999999999998</v>
+      </c>
+      <c r="D28">
+        <v>88.31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>50.149253999999999</v>
+      </c>
+      <c r="B29">
+        <v>50.554772999999997</v>
+      </c>
+      <c r="C29">
+        <v>2.25</v>
+      </c>
+      <c r="D29">
+        <v>89.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>50.554772999999997</v>
+      </c>
+      <c r="B30">
+        <v>50.965924999999999</v>
+      </c>
+      <c r="C30">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="D30">
+        <v>89.76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>50.965924999999999</v>
+      </c>
+      <c r="B31">
+        <v>51.371445000000001</v>
+      </c>
+      <c r="C31">
+        <v>2.4169999999999998</v>
+      </c>
+      <c r="D31">
+        <v>90.49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>51.371445000000001</v>
+      </c>
+      <c r="B32">
+        <v>51.776964</v>
+      </c>
+      <c r="C32">
+        <v>2.5</v>
+      </c>
+      <c r="D32">
+        <v>91.21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>51.776964</v>
+      </c>
+      <c r="B33">
+        <v>52.182484000000002</v>
+      </c>
+      <c r="C33">
+        <v>2.5830000000000002</v>
+      </c>
+      <c r="D33">
+        <v>91.93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>52.182484000000002</v>
+      </c>
+      <c r="B34">
+        <v>52.582371000000002</v>
+      </c>
+      <c r="C34">
+        <v>2.6669999999999998</v>
+      </c>
+      <c r="D34">
+        <v>92.65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>52.582371000000002</v>
+      </c>
+      <c r="B35">
+        <v>52.970993999999997</v>
+      </c>
+      <c r="C35">
+        <v>2.75</v>
+      </c>
+      <c r="D35">
+        <v>93.36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>52.970993999999997</v>
+      </c>
+      <c r="B36">
+        <v>53.359617</v>
+      </c>
+      <c r="C36">
+        <v>2.8330000000000002</v>
+      </c>
+      <c r="D36">
+        <v>94.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>53.359617</v>
+      </c>
+      <c r="B37">
+        <v>53.736975000000001</v>
+      </c>
+      <c r="C37">
+        <v>2.9169999999999998</v>
+      </c>
+      <c r="D37">
+        <v>94.74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>53.736975000000001</v>
+      </c>
+      <c r="B38">
+        <v>54.103070000000002</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>95.41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>54.103070000000002</v>
+      </c>
+      <c r="B39">
+        <v>54.463531000000003</v>
+      </c>
+      <c r="C39">
+        <v>3.0830000000000002</v>
+      </c>
+      <c r="D39">
+        <v>96.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>54.463531000000003</v>
+      </c>
+      <c r="B40">
+        <v>54.812728999999997</v>
+      </c>
+      <c r="C40">
+        <v>3.1669999999999998</v>
+      </c>
+      <c r="D40">
+        <v>96.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>54.812728999999997</v>
+      </c>
+      <c r="B41">
+        <v>55.156294000000003</v>
+      </c>
+      <c r="C41">
+        <v>3.25</v>
+      </c>
+      <c r="D41">
+        <v>97.32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>55.156294000000003</v>
+      </c>
+      <c r="B42">
+        <v>55.494227000000002</v>
+      </c>
+      <c r="C42">
+        <v>3.3330000000000002</v>
+      </c>
+      <c r="D42">
+        <v>97.93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>55.494227000000002</v>
+      </c>
+      <c r="B43">
+        <v>55.820895999999998</v>
+      </c>
+      <c r="C43">
+        <v>3.4169999999999998</v>
+      </c>
+      <c r="D43">
+        <v>98.53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>55.820895999999998</v>
+      </c>
+      <c r="B44">
+        <v>56.147564000000003</v>
+      </c>
+      <c r="C44">
+        <v>3.5</v>
+      </c>
+      <c r="D44">
+        <v>99.11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>56.147564000000003</v>
+      </c>
+      <c r="B45">
+        <v>56.462967999999996</v>
+      </c>
+      <c r="C45">
+        <v>3.5830000000000002</v>
+      </c>
+      <c r="D45">
+        <v>99.69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>56.462967999999996</v>
+      </c>
+      <c r="B46">
+        <v>56.778371999999997</v>
+      </c>
+      <c r="C46">
+        <v>3.6669999999999998</v>
+      </c>
+      <c r="D46">
+        <v>100.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>56.778371999999997</v>
+      </c>
+      <c r="B47">
+        <v>57.093775999999998</v>
+      </c>
+      <c r="C47">
+        <v>3.75</v>
+      </c>
+      <c r="D47">
+        <v>100.81</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>57.093775999999998</v>
+      </c>
+      <c r="B48">
+        <v>57.409180999999997</v>
+      </c>
+      <c r="C48">
+        <v>3.8330000000000002</v>
+      </c>
+      <c r="D48">
+        <v>101.37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>57.409180999999997</v>
+      </c>
+      <c r="B49">
+        <v>57.724584999999998</v>
+      </c>
+      <c r="C49">
+        <v>3.9169999999999998</v>
+      </c>
+      <c r="D49">
+        <v>101.93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>57.724584999999998</v>
+      </c>
+      <c r="B50">
+        <v>58.045620999999997</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>102.49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>58.045620999999997</v>
+      </c>
+      <c r="B51">
+        <v>58.372289000000002</v>
+      </c>
+      <c r="C51">
+        <v>4.0830000000000002</v>
+      </c>
+      <c r="D51">
+        <v>103.06</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>58.372289000000002</v>
+      </c>
+      <c r="B52">
+        <v>58.698957999999998</v>
+      </c>
+      <c r="C52">
+        <v>4.1669999999999998</v>
+      </c>
+      <c r="D52">
+        <v>103.64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>58.698957999999998</v>
+      </c>
+      <c r="B53">
+        <v>59.025627</v>
+      </c>
+      <c r="C53">
+        <v>4.25</v>
+      </c>
+      <c r="D53">
+        <v>104.22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>59.025627</v>
+      </c>
+      <c r="B54">
+        <v>59.36356</v>
+      </c>
+      <c r="C54">
+        <v>4.3330000000000002</v>
+      </c>
+      <c r="D54">
+        <v>104.8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>59.36356</v>
+      </c>
+      <c r="B55">
+        <v>59.701492999999999</v>
+      </c>
+      <c r="C55">
+        <v>4.4169999999999998</v>
+      </c>
+      <c r="D55">
+        <v>105.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>59.701492999999999</v>
+      </c>
+      <c r="B56">
+        <v>60.039425999999999</v>
+      </c>
+      <c r="C56">
+        <v>4.5</v>
+      </c>
+      <c r="D56">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>60.039425999999999</v>
+      </c>
+      <c r="B57">
+        <v>60.382990999999997</v>
+      </c>
+      <c r="C57">
+        <v>4.5830000000000002</v>
+      </c>
+      <c r="D57">
+        <v>106.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>60.382990999999997</v>
+      </c>
+      <c r="B58">
+        <v>60.720923999999997</v>
+      </c>
+      <c r="C58">
+        <v>4.6669999999999998</v>
+      </c>
+      <c r="D58">
+        <v>107.21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>60.720923999999997</v>
+      </c>
+      <c r="B59">
+        <v>61.058857000000003</v>
+      </c>
+      <c r="C59">
+        <v>4.75</v>
+      </c>
+      <c r="D59">
+        <v>107.81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>61.058857000000003</v>
+      </c>
+      <c r="B60">
+        <v>61.396790000000003</v>
+      </c>
+      <c r="C60">
+        <v>4.8330000000000002</v>
+      </c>
+      <c r="D60">
+        <v>108.41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>61.396790000000003</v>
+      </c>
+      <c r="B61">
+        <v>61.723458000000001</v>
+      </c>
+      <c r="C61">
+        <v>4.9169999999999998</v>
+      </c>
+      <c r="D61">
+        <v>109.01</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61.723458000000001</v>
+      </c>
+      <c r="B62">
+        <v>62.044494999999998</v>
+      </c>
+      <c r="C62">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>109.59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62.044494999999998</v>
+      </c>
+      <c r="B63">
+        <v>62.365530999999997</v>
+      </c>
+      <c r="C63">
+        <v>5.0830000000000002</v>
+      </c>
+      <c r="D63">
+        <v>110.16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>62.365530999999997</v>
+      </c>
+      <c r="B64">
+        <v>62.675303</v>
+      </c>
+      <c r="C64">
+        <v>5.1669999999999998</v>
+      </c>
+      <c r="D64">
+        <v>110.73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>62.675303</v>
+      </c>
+      <c r="B65">
+        <v>62.97381</v>
+      </c>
+      <c r="C65">
+        <v>5.25</v>
+      </c>
+      <c r="D65">
+        <v>111.28</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>62.97381</v>
+      </c>
+      <c r="B66">
+        <v>63.277949999999997</v>
+      </c>
+      <c r="C66">
+        <v>5.3330000000000002</v>
+      </c>
+      <c r="D66">
+        <v>111.81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>63.277949999999997</v>
+      </c>
+      <c r="B67">
+        <v>63.570824999999999</v>
+      </c>
+      <c r="C67">
+        <v>5.4169999999999998</v>
+      </c>
+      <c r="D67">
+        <v>112.35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>63.570824999999999</v>
+      </c>
+      <c r="B68">
+        <v>63.858068000000003</v>
+      </c>
+      <c r="C68">
+        <v>5.5</v>
+      </c>
+      <c r="D68">
+        <v>112.87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>63.858068000000003</v>
+      </c>
+      <c r="B69">
+        <v>64.150942999999998</v>
+      </c>
+      <c r="C69">
+        <v>5.5830000000000002</v>
+      </c>
+      <c r="D69">
+        <v>113.38</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>64.150942999999998</v>
+      </c>
+      <c r="B70">
+        <v>64.438186000000002</v>
+      </c>
+      <c r="C70">
+        <v>5.6669999999999998</v>
+      </c>
+      <c r="D70">
+        <v>113.9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>64.438186000000002</v>
+      </c>
+      <c r="B71">
+        <v>64.725429000000005</v>
+      </c>
+      <c r="C71">
+        <v>5.75</v>
+      </c>
+      <c r="D71">
+        <v>114.41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>64.725429000000005</v>
+      </c>
+      <c r="B72">
+        <v>65.012671999999995</v>
+      </c>
+      <c r="C72">
+        <v>5.8330000000000002</v>
+      </c>
+      <c r="D72">
+        <v>114.92</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>65.012671999999995</v>
+      </c>
+      <c r="B73">
+        <v>65.294282999999993</v>
+      </c>
+      <c r="C73">
+        <v>5.9169999999999998</v>
+      </c>
+      <c r="D73">
+        <v>115.43</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>65.294282999999993</v>
+      </c>
+      <c r="B74">
+        <v>65.581525999999997</v>
+      </c>
+      <c r="C74">
+        <v>6</v>
+      </c>
+      <c r="D74">
+        <v>115.93</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>65.581525999999997</v>
+      </c>
+      <c r="B75">
+        <v>65.863136999999995</v>
+      </c>
+      <c r="C75">
+        <v>6.0830000000000002</v>
+      </c>
+      <c r="D75">
+        <v>116.44</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>65.863136999999995</v>
+      </c>
+      <c r="B76">
+        <v>66.144748000000007</v>
+      </c>
+      <c r="C76">
+        <v>6.1669999999999998</v>
+      </c>
+      <c r="D76">
+        <v>116.94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>66.144748000000007</v>
+      </c>
+      <c r="B77">
+        <v>66.426359000000005</v>
+      </c>
+      <c r="C77">
+        <v>6.25</v>
+      </c>
+      <c r="D77">
+        <v>117.44</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>66.426359000000005</v>
+      </c>
+      <c r="B78">
+        <v>66.702337</v>
+      </c>
+      <c r="C78">
+        <v>6.3330000000000002</v>
+      </c>
+      <c r="D78">
+        <v>117.94</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>66.702337</v>
+      </c>
+      <c r="B79">
+        <v>66.983947999999998</v>
+      </c>
+      <c r="C79">
+        <v>6.4169999999999998</v>
+      </c>
+      <c r="D79">
+        <v>118.43</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>66.983947999999998</v>
+      </c>
+      <c r="B80">
+        <v>67.259927000000005</v>
+      </c>
+      <c r="C80">
+        <v>6.5</v>
+      </c>
+      <c r="D80">
+        <v>118.93</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>67.259927000000005</v>
+      </c>
+      <c r="B81">
+        <v>67.535905</v>
+      </c>
+      <c r="C81">
+        <v>6.5830000000000002</v>
+      </c>
+      <c r="D81">
+        <v>119.42</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>67.535905</v>
+      </c>
+      <c r="B82">
+        <v>67.817515999999998</v>
+      </c>
+      <c r="C82">
+        <v>6.6669999999999998</v>
+      </c>
+      <c r="D82">
+        <v>119.91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>67.817515999999998</v>
+      </c>
+      <c r="B83">
+        <v>68.093495000000004</v>
+      </c>
+      <c r="C83">
+        <v>6.75</v>
+      </c>
+      <c r="D83">
+        <v>120.41</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>68.093495000000004</v>
+      </c>
+      <c r="B84">
+        <v>68.375106000000002</v>
+      </c>
+      <c r="C84">
+        <v>6.8330000000000002</v>
+      </c>
+      <c r="D84">
+        <v>120.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>68.375106000000002</v>
+      </c>
+      <c r="B85">
+        <v>68.656716000000003</v>
+      </c>
+      <c r="C85">
+        <v>6.9169999999999998</v>
+      </c>
+      <c r="D85">
+        <v>121.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>68.656716000000003</v>
+      </c>
+      <c r="B86">
+        <v>68.938327000000001</v>
+      </c>
+      <c r="C86">
+        <v>7</v>
+      </c>
+      <c r="D86">
+        <v>121.9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>68.938327000000001</v>
+      </c>
+      <c r="B87">
+        <v>69.219937999999999</v>
+      </c>
+      <c r="C87">
+        <v>7.0830000000000002</v>
+      </c>
+      <c r="D87">
+        <v>122.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>69.219937999999999</v>
+      </c>
+      <c r="B88">
+        <v>69.501548999999997</v>
+      </c>
+      <c r="C88">
+        <v>7.1669999999999998</v>
+      </c>
+      <c r="D88">
+        <v>122.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>69.501548999999997</v>
+      </c>
+      <c r="B89">
+        <v>69.783159999999995</v>
+      </c>
+      <c r="C89">
+        <v>7.25</v>
+      </c>
+      <c r="D89">
+        <v>123.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>69.783159999999995</v>
+      </c>
+      <c r="B90">
+        <v>70.064769999999996</v>
+      </c>
+      <c r="C90">
+        <v>7.3330000000000002</v>
+      </c>
+      <c r="D90">
+        <v>123.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>70.064769999999996</v>
+      </c>
+      <c r="B91">
+        <v>70.346380999999994</v>
+      </c>
+      <c r="C91">
+        <v>7.4169999999999998</v>
+      </c>
+      <c r="D91">
+        <v>124.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>70.346380999999994</v>
+      </c>
+      <c r="B92">
+        <v>70.627992000000006</v>
+      </c>
+      <c r="C92">
+        <v>7.5</v>
+      </c>
+      <c r="D92">
+        <v>124.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>70.627992000000006</v>
+      </c>
+      <c r="B93">
+        <v>70.903970999999999</v>
+      </c>
+      <c r="C93">
+        <v>7.5830000000000002</v>
+      </c>
+      <c r="D93">
+        <v>125.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>70.903970999999999</v>
+      </c>
+      <c r="B94">
+        <v>71.185581999999997</v>
+      </c>
+      <c r="C94">
+        <v>7.6669999999999998</v>
+      </c>
+      <c r="D94">
+        <v>125.89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>71.185581999999997</v>
+      </c>
+      <c r="B95">
+        <v>71.455928</v>
+      </c>
+      <c r="C95">
+        <v>7.75</v>
+      </c>
+      <c r="D95">
+        <v>126.39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>71.455928</v>
+      </c>
+      <c r="B96">
+        <v>71.731907000000007</v>
+      </c>
+      <c r="C96">
+        <v>7.8330000000000002</v>
+      </c>
+      <c r="D96">
+        <v>126.87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>71.731907000000007</v>
+      </c>
+      <c r="B97">
+        <v>72.007885000000002</v>
+      </c>
+      <c r="C97">
+        <v>7.9169999999999998</v>
+      </c>
+      <c r="D97">
+        <v>127.36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>72.007885000000002</v>
+      </c>
+      <c r="B98">
+        <v>72.278231000000005</v>
+      </c>
+      <c r="C98">
+        <v>8</v>
+      </c>
+      <c r="D98">
+        <v>127.85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>72.278231000000005</v>
+      </c>
+      <c r="B99">
+        <v>72.542946000000001</v>
+      </c>
+      <c r="C99">
+        <v>8.0830000000000002</v>
+      </c>
+      <c r="D99">
+        <v>128.33000000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>72.542946000000001</v>
+      </c>
+      <c r="B100">
+        <v>72.807659999999998</v>
+      </c>
+      <c r="C100">
+        <v>8.1669999999999998</v>
+      </c>
+      <c r="D100">
+        <v>128.80000000000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>72.807659999999998</v>
+      </c>
+      <c r="B101">
+        <v>73.072373999999996</v>
+      </c>
+      <c r="C101">
+        <v>8.25</v>
+      </c>
+      <c r="D101">
+        <v>129.27000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>73.072373999999996</v>
+      </c>
+      <c r="B102">
+        <v>73.325823999999997</v>
+      </c>
+      <c r="C102">
+        <v>8.3330000000000002</v>
+      </c>
+      <c r="D102">
+        <v>129.74</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>73.325823999999997</v>
+      </c>
+      <c r="B103">
+        <v>73.579273000000001</v>
+      </c>
+      <c r="C103">
+        <v>8.4169999999999998</v>
+      </c>
+      <c r="D103">
+        <v>130.19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>73.579273000000001</v>
+      </c>
+      <c r="B104">
+        <v>73.832723000000001</v>
+      </c>
+      <c r="C104">
+        <v>8.5</v>
+      </c>
+      <c r="D104">
+        <v>130.63999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>73.832723000000001</v>
+      </c>
+      <c r="B105">
+        <v>74.086173000000002</v>
+      </c>
+      <c r="C105">
+        <v>8.5830000000000002</v>
+      </c>
+      <c r="D105">
+        <v>131.09</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>74.086173000000002</v>
+      </c>
+      <c r="B106">
+        <v>74.328357999999994</v>
+      </c>
+      <c r="C106">
+        <v>8.6669999999999998</v>
+      </c>
+      <c r="D106">
+        <v>131.54</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>74.328357999999994</v>
+      </c>
+      <c r="B107">
+        <v>74.576176000000004</v>
+      </c>
+      <c r="C107">
+        <v>8.75</v>
+      </c>
+      <c r="D107">
+        <v>131.97</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>74.576176000000004</v>
+      </c>
+      <c r="B108">
+        <v>74.818360999999996</v>
+      </c>
+      <c r="C108">
+        <v>8.8330000000000002</v>
+      </c>
+      <c r="D108">
+        <v>132.41</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>74.818360999999996</v>
+      </c>
+      <c r="B109">
+        <v>75.066179000000005</v>
+      </c>
+      <c r="C109">
+        <v>8.9169999999999998</v>
+      </c>
+      <c r="D109">
+        <v>132.84</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>75.066179000000005</v>
+      </c>
+      <c r="B110">
+        <v>75.308363999999997</v>
+      </c>
+      <c r="C110">
+        <v>9</v>
+      </c>
+      <c r="D110">
+        <v>133.28</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>75.308363999999997</v>
+      </c>
+      <c r="B111">
+        <v>75.550549000000004</v>
+      </c>
+      <c r="C111">
+        <v>9.0830000000000002</v>
+      </c>
+      <c r="D111">
+        <v>133.71</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>75.550549000000004</v>
+      </c>
+      <c r="B112">
+        <v>75.792733999999996</v>
+      </c>
+      <c r="C112">
+        <v>9.1669999999999998</v>
+      </c>
+      <c r="D112">
+        <v>134.13999999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>75.792733999999996</v>
+      </c>
+      <c r="B113">
+        <v>76.029287999999994</v>
+      </c>
+      <c r="C113">
+        <v>9.25</v>
+      </c>
+      <c r="D113">
+        <v>134.57</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>76.029287999999994</v>
+      </c>
+      <c r="B114">
+        <v>76.271473</v>
+      </c>
+      <c r="C114">
+        <v>9.3330000000000002</v>
+      </c>
+      <c r="D114">
+        <v>134.99</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>76.271473</v>
+      </c>
+      <c r="B115">
+        <v>76.508026000000001</v>
+      </c>
+      <c r="C115">
+        <v>9.4169999999999998</v>
+      </c>
+      <c r="D115">
+        <v>135.41999999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>76.508026000000001</v>
+      </c>
+      <c r="B116">
+        <v>76.744579000000002</v>
+      </c>
+      <c r="C116">
+        <v>9.5</v>
+      </c>
+      <c r="D116">
+        <v>135.84</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>76.744579000000002</v>
+      </c>
+      <c r="B117">
+        <v>76.981132000000002</v>
+      </c>
+      <c r="C117">
+        <v>9.5830000000000002</v>
+      </c>
+      <c r="D117">
+        <v>136.26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>76.981132000000002</v>
+      </c>
+      <c r="B118">
+        <v>77.217685000000003</v>
+      </c>
+      <c r="C118">
+        <v>9.6669999999999998</v>
+      </c>
+      <c r="D118">
+        <v>136.68</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>77.217685000000003</v>
+      </c>
+      <c r="B119">
+        <v>77.459869999999995</v>
+      </c>
+      <c r="C119">
+        <v>9.75</v>
+      </c>
+      <c r="D119">
+        <v>137.1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>77.459869999999995</v>
+      </c>
+      <c r="B120">
+        <v>77.702055999999999</v>
+      </c>
+      <c r="C120">
+        <v>9.8330000000000002</v>
+      </c>
+      <c r="D120">
+        <v>137.53</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>77.702055999999999</v>
+      </c>
+      <c r="B121">
+        <v>77.944241000000005</v>
+      </c>
+      <c r="C121">
+        <v>9.9169999999999998</v>
+      </c>
+      <c r="D121">
+        <v>137.96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>77.944241000000005</v>
+      </c>
+      <c r="B122">
+        <v>78.186425999999997</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+      <c r="D122">
+        <v>138.38999999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>78.186425999999997</v>
+      </c>
+      <c r="B123">
+        <v>78.434244000000007</v>
+      </c>
+      <c r="C123">
+        <v>10.083</v>
+      </c>
+      <c r="D123">
+        <v>138.82</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>78.434244000000007</v>
+      </c>
+      <c r="B124">
+        <v>78.676428999999999</v>
+      </c>
+      <c r="C124">
+        <v>10.167</v>
+      </c>
+      <c r="D124">
+        <v>139.26</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>78.676428999999999</v>
+      </c>
+      <c r="B125">
+        <v>78.918614000000005</v>
+      </c>
+      <c r="C125">
+        <v>10.25</v>
+      </c>
+      <c r="D125">
+        <v>139.69</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>78.918614000000005</v>
+      </c>
+      <c r="B126">
+        <v>79.155168000000003</v>
+      </c>
+      <c r="C126">
+        <v>10.333</v>
+      </c>
+      <c r="D126">
+        <v>140.12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>79.155168000000003</v>
+      </c>
+      <c r="B127">
+        <v>79.391721000000004</v>
+      </c>
+      <c r="C127">
+        <v>10.417</v>
+      </c>
+      <c r="D127">
+        <v>140.54</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>79.391721000000004</v>
+      </c>
+      <c r="B128">
+        <v>79.622641999999999</v>
+      </c>
+      <c r="C128">
+        <v>10.5</v>
+      </c>
+      <c r="D128">
+        <v>140.96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>79.622641999999999</v>
+      </c>
+      <c r="B129">
+        <v>79.853561999999997</v>
+      </c>
+      <c r="C129">
+        <v>10.583</v>
+      </c>
+      <c r="D129">
+        <v>141.37</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>79.853561999999997</v>
+      </c>
+      <c r="B130">
+        <v>80.078851</v>
+      </c>
+      <c r="C130">
+        <v>10.667</v>
+      </c>
+      <c r="D130">
+        <v>141.78</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>80.078851</v>
+      </c>
+      <c r="B131">
+        <v>80.304140000000004</v>
+      </c>
+      <c r="C131">
+        <v>10.75</v>
+      </c>
+      <c r="D131">
+        <v>142.18</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>80.304140000000004</v>
+      </c>
+      <c r="B132">
+        <v>80.529427999999996</v>
+      </c>
+      <c r="C132">
+        <v>10.833</v>
+      </c>
+      <c r="D132">
+        <v>142.58000000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>80.529427999999996</v>
+      </c>
+      <c r="B133">
+        <v>80.749084999999994</v>
+      </c>
+      <c r="C133">
+        <v>10.917</v>
+      </c>
+      <c r="D133">
+        <v>142.97999999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>80.749084999999994</v>
+      </c>
+      <c r="B134">
+        <v>80.974373</v>
+      </c>
+      <c r="C134">
+        <v>11</v>
+      </c>
+      <c r="D134">
+        <v>143.37</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>80.974373</v>
+      </c>
+      <c r="B135">
+        <v>81.194029999999998</v>
+      </c>
+      <c r="C135">
+        <v>11.083</v>
+      </c>
+      <c r="D135">
+        <v>143.77000000000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>81.194029999999998</v>
+      </c>
+      <c r="B136">
+        <v>81.413685999999998</v>
+      </c>
+      <c r="C136">
+        <v>11.167</v>
+      </c>
+      <c r="D136">
+        <v>144.16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>81.413685999999998</v>
+      </c>
+      <c r="B137">
+        <v>81.638975000000002</v>
+      </c>
+      <c r="C137">
+        <v>11.25</v>
+      </c>
+      <c r="D137">
+        <v>144.55000000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>81.638975000000002</v>
+      </c>
+      <c r="B138">
+        <v>81.858631000000003</v>
+      </c>
+      <c r="C138">
+        <v>11.333</v>
+      </c>
+      <c r="D138">
+        <v>144.94999999999999</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>81.858631000000003</v>
+      </c>
+      <c r="B139">
+        <v>82.089551999999998</v>
+      </c>
+      <c r="C139">
+        <v>11.417</v>
+      </c>
+      <c r="D139">
+        <v>145.34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>82.089551999999998</v>
+      </c>
+      <c r="B140">
+        <v>82.320473000000007</v>
+      </c>
+      <c r="C140">
+        <v>11.5</v>
+      </c>
+      <c r="D140">
+        <v>145.75</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>82.320473000000007</v>
+      </c>
+      <c r="B141">
+        <v>82.557025999999993</v>
+      </c>
+      <c r="C141">
+        <v>11.583</v>
+      </c>
+      <c r="D141">
+        <v>146.16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>82.557025999999993</v>
+      </c>
+      <c r="B142">
+        <v>82.804844000000003</v>
+      </c>
+      <c r="C142">
+        <v>11.667</v>
+      </c>
+      <c r="D142">
+        <v>146.58000000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>82.804844000000003</v>
+      </c>
+      <c r="B143">
+        <v>83.052661000000001</v>
+      </c>
+      <c r="C143">
+        <v>11.75</v>
+      </c>
+      <c r="D143">
+        <v>147.02000000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>83.052661000000001</v>
+      </c>
+      <c r="B144">
+        <v>83.306111000000001</v>
+      </c>
+      <c r="C144">
+        <v>11.833</v>
+      </c>
+      <c r="D144">
+        <v>147.46</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>83.306111000000001</v>
+      </c>
+      <c r="B145">
+        <v>83.559561000000002</v>
+      </c>
+      <c r="C145">
+        <v>11.917</v>
+      </c>
+      <c r="D145">
+        <v>147.91</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>83.559561000000002</v>
+      </c>
+      <c r="B146">
+        <v>83.824275</v>
+      </c>
+      <c r="C146">
+        <v>12</v>
+      </c>
+      <c r="D146">
+        <v>148.36000000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>83.824275</v>
+      </c>
+      <c r="B147">
+        <v>84.094621000000004</v>
+      </c>
+      <c r="C147">
+        <v>12.083</v>
+      </c>
+      <c r="D147">
+        <v>148.83000000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>84.094621000000004</v>
+      </c>
+      <c r="B148">
+        <v>84.376232000000002</v>
+      </c>
+      <c r="C148">
+        <v>12.167</v>
+      </c>
+      <c r="D148">
+        <v>149.31</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>84.376232000000002</v>
+      </c>
+      <c r="B149">
+        <v>84.657843</v>
+      </c>
+      <c r="C149">
+        <v>12.25</v>
+      </c>
+      <c r="D149">
+        <v>149.81</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>84.657843</v>
+      </c>
+      <c r="B150">
+        <v>84.950717999999995</v>
+      </c>
+      <c r="C150">
+        <v>12.333</v>
+      </c>
+      <c r="D150">
+        <v>150.31</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>84.950717999999995</v>
+      </c>
+      <c r="B151">
+        <v>85.243593000000004</v>
+      </c>
+      <c r="C151">
+        <v>12.417</v>
+      </c>
+      <c r="D151">
+        <v>150.83000000000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>85.243593000000004</v>
+      </c>
+      <c r="B152">
+        <v>85.547732999999994</v>
+      </c>
+      <c r="C152">
+        <v>12.5</v>
+      </c>
+      <c r="D152">
+        <v>151.35</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>85.547732999999994</v>
+      </c>
+      <c r="B153">
+        <v>85.857505000000003</v>
+      </c>
+      <c r="C153">
+        <v>12.583</v>
+      </c>
+      <c r="D153">
+        <v>151.88999999999999</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>85.857505000000003</v>
+      </c>
+      <c r="B154">
+        <v>86.172909000000004</v>
+      </c>
+      <c r="C154">
+        <v>12.667</v>
+      </c>
+      <c r="D154">
+        <v>152.44</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>86.172909000000004</v>
+      </c>
+      <c r="B155">
+        <v>86.499578</v>
+      </c>
+      <c r="C155">
+        <v>12.75</v>
+      </c>
+      <c r="D155">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>86.499578</v>
+      </c>
+      <c r="B156">
+        <v>86.831878000000003</v>
+      </c>
+      <c r="C156">
+        <v>12.833</v>
+      </c>
+      <c r="D156">
+        <v>153.58000000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>86.831878000000003</v>
+      </c>
+      <c r="B157">
+        <v>87.169810999999996</v>
+      </c>
+      <c r="C157">
+        <v>12.917</v>
+      </c>
+      <c r="D157">
+        <v>154.16999999999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>87.169810999999996</v>
+      </c>
+      <c r="B158">
+        <v>87.513377000000006</v>
+      </c>
+      <c r="C158">
+        <v>13</v>
+      </c>
+      <c r="D158">
+        <v>154.77000000000001</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>87.513377000000006</v>
+      </c>
+      <c r="B159">
+        <v>87.862573999999995</v>
+      </c>
+      <c r="C159">
+        <v>13.083</v>
+      </c>
+      <c r="D159">
+        <v>155.38</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>87.862573999999995</v>
+      </c>
+      <c r="B160">
+        <v>88.217404000000002</v>
+      </c>
+      <c r="C160">
+        <v>13.167</v>
+      </c>
+      <c r="D160">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>88.217404000000002</v>
+      </c>
+      <c r="B161">
+        <v>88.577865000000003</v>
+      </c>
+      <c r="C161">
+        <v>13.25</v>
+      </c>
+      <c r="D161">
+        <v>156.63</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>88.577865000000003</v>
+      </c>
+      <c r="B162">
+        <v>88.938327000000001</v>
+      </c>
+      <c r="C162">
+        <v>13.333</v>
+      </c>
+      <c r="D162">
+        <v>157.27000000000001</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>88.938327000000001</v>
+      </c>
+      <c r="B163">
+        <v>89.298788999999999</v>
+      </c>
+      <c r="C163">
+        <v>13.417</v>
+      </c>
+      <c r="D163">
+        <v>157.91</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>89.298788999999999</v>
+      </c>
+      <c r="B164">
+        <v>89.664883000000003</v>
+      </c>
+      <c r="C164">
+        <v>13.5</v>
+      </c>
+      <c r="D164">
+        <v>158.55000000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>89.664883000000003</v>
+      </c>
+      <c r="B165">
+        <v>90.025345000000002</v>
+      </c>
+      <c r="C165">
+        <v>13.583</v>
+      </c>
+      <c r="D165">
+        <v>159.19999999999999</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>90.025345000000002</v>
+      </c>
+      <c r="B166">
+        <v>90.380174999999994</v>
+      </c>
+      <c r="C166">
+        <v>13.667</v>
+      </c>
+      <c r="D166">
+        <v>159.84</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>90.380174999999994</v>
+      </c>
+      <c r="B167">
+        <v>90.740635999999995</v>
+      </c>
+      <c r="C167">
+        <v>13.75</v>
+      </c>
+      <c r="D167">
+        <v>160.47</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>90.740635999999995</v>
+      </c>
+      <c r="B168">
+        <v>91.095466000000002</v>
+      </c>
+      <c r="C168">
+        <v>13.833</v>
+      </c>
+      <c r="D168">
+        <v>161.11000000000001</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>91.095466000000002</v>
+      </c>
+      <c r="B169">
+        <v>91.444663000000006</v>
+      </c>
+      <c r="C169">
+        <v>13.917</v>
+      </c>
+      <c r="D169">
+        <v>161.74</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>91.444663000000006</v>
+      </c>
+      <c r="B170">
+        <v>91.788229000000001</v>
+      </c>
+      <c r="C170">
+        <v>14</v>
+      </c>
+      <c r="D170">
+        <v>162.36000000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>91.788229000000001</v>
+      </c>
+      <c r="B171">
+        <v>92.131793999999999</v>
+      </c>
+      <c r="C171">
+        <v>14.083</v>
+      </c>
+      <c r="D171">
+        <v>162.97</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>92.131793999999999</v>
+      </c>
+      <c r="B172">
+        <v>92.464095</v>
+      </c>
+      <c r="C172">
+        <v>14.167</v>
+      </c>
+      <c r="D172">
+        <v>163.58000000000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>92.464095</v>
+      </c>
+      <c r="B173">
+        <v>92.790762999999998</v>
+      </c>
+      <c r="C173">
+        <v>14.25</v>
+      </c>
+      <c r="D173">
+        <v>164.17</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>92.790762999999998</v>
+      </c>
+      <c r="B174">
+        <v>93.117431999999994</v>
+      </c>
+      <c r="C174">
+        <v>14.333</v>
+      </c>
+      <c r="D174">
+        <v>164.75</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>93.117431999999994</v>
+      </c>
+      <c r="B175">
+        <v>93.427204000000003</v>
+      </c>
+      <c r="C175">
+        <v>14.417</v>
+      </c>
+      <c r="D175">
+        <v>165.33</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>93.427204000000003</v>
+      </c>
+      <c r="B176">
+        <v>93.736975000000001</v>
+      </c>
+      <c r="C176">
+        <v>14.5</v>
+      </c>
+      <c r="D176">
+        <v>165.88</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>93.736975000000001</v>
+      </c>
+      <c r="B177">
+        <v>94.035482999999999</v>
+      </c>
+      <c r="C177">
+        <v>14.583</v>
+      </c>
+      <c r="D177">
+        <v>166.43</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>94.035482999999999</v>
+      </c>
+      <c r="B178">
+        <v>94.328357999999994</v>
+      </c>
+      <c r="C178">
+        <v>14.667</v>
+      </c>
+      <c r="D178">
+        <v>166.96</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>94.328357999999994</v>
+      </c>
+      <c r="B179">
+        <v>94.609969000000007</v>
+      </c>
+      <c r="C179">
+        <v>14.75</v>
+      </c>
+      <c r="D179">
+        <v>167.48</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>94.609969000000007</v>
+      </c>
+      <c r="B180">
+        <v>94.885947999999999</v>
+      </c>
+      <c r="C180">
+        <v>14.833</v>
+      </c>
+      <c r="D180">
+        <v>167.98</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>94.885947999999999</v>
+      </c>
+      <c r="B181">
+        <v>95.150661999999997</v>
+      </c>
+      <c r="C181">
+        <v>14.917</v>
+      </c>
+      <c r="D181">
+        <v>168.47</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>95.150661999999997</v>
+      </c>
+      <c r="B182">
+        <v>95.409744000000003</v>
+      </c>
+      <c r="C182">
+        <v>15</v>
+      </c>
+      <c r="D182">
+        <v>168.94</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>95.409744000000003</v>
+      </c>
+      <c r="B183">
+        <v>95.657561000000001</v>
+      </c>
+      <c r="C183">
+        <v>15.083</v>
+      </c>
+      <c r="D183">
+        <v>169.4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>95.657561000000001</v>
+      </c>
+      <c r="B184">
+        <v>95.894114000000002</v>
+      </c>
+      <c r="C184">
+        <v>15.167</v>
+      </c>
+      <c r="D184">
+        <v>169.84</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>95.894114000000002</v>
+      </c>
+      <c r="B185">
+        <v>96.125034999999997</v>
+      </c>
+      <c r="C185">
+        <v>15.25</v>
+      </c>
+      <c r="D185">
+        <v>170.26</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>96.125034999999997</v>
+      </c>
+      <c r="B186">
+        <v>96.344691999999995</v>
+      </c>
+      <c r="C186">
+        <v>15.333</v>
+      </c>
+      <c r="D186">
+        <v>170.67</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>96.344691999999995</v>
+      </c>
+      <c r="B187">
+        <v>96.553083999999998</v>
+      </c>
+      <c r="C187">
+        <v>15.417</v>
+      </c>
+      <c r="D187">
+        <v>171.06</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>96.553083999999998</v>
+      </c>
+      <c r="B188">
+        <v>96.755842999999999</v>
+      </c>
+      <c r="C188">
+        <v>15.5</v>
+      </c>
+      <c r="D188">
+        <v>171.43</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>96.755842999999999</v>
+      </c>
+      <c r="B189">
+        <v>96.952971000000005</v>
+      </c>
+      <c r="C189">
+        <v>15.583</v>
+      </c>
+      <c r="D189">
+        <v>171.79</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>96.952971000000005</v>
+      </c>
+      <c r="B190">
+        <v>97.144465999999994</v>
+      </c>
+      <c r="C190">
+        <v>15.667</v>
+      </c>
+      <c r="D190">
+        <v>172.14</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>97.144465999999994</v>
+      </c>
+      <c r="B191">
+        <v>97.319064999999995</v>
+      </c>
+      <c r="C191">
+        <v>15.75</v>
+      </c>
+      <c r="D191">
+        <v>172.48</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>97.319064999999995</v>
+      </c>
+      <c r="B192">
+        <v>97.493663999999995</v>
+      </c>
+      <c r="C192">
+        <v>15.833</v>
+      </c>
+      <c r="D192">
+        <v>172.79</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>97.493663999999995</v>
+      </c>
+      <c r="B193">
+        <v>97.656998000000002</v>
+      </c>
+      <c r="C193">
+        <v>15.917</v>
+      </c>
+      <c r="D193">
+        <v>173.1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>97.656998000000002</v>
+      </c>
+      <c r="B194">
+        <v>97.809067999999996</v>
+      </c>
+      <c r="C194">
+        <v>16</v>
+      </c>
+      <c r="D194">
+        <v>173.39</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>97.809067999999996</v>
+      </c>
+      <c r="B195">
+        <v>97.961138000000005</v>
+      </c>
+      <c r="C195">
+        <v>16.082999999999998</v>
+      </c>
+      <c r="D195">
+        <v>173.66</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>97.961138000000005</v>
+      </c>
+      <c r="B196">
+        <v>98.101943000000006</v>
+      </c>
+      <c r="C196">
+        <v>16.167000000000002</v>
+      </c>
+      <c r="D196">
+        <v>173.93</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>98.101943000000006</v>
+      </c>
+      <c r="B197">
+        <v>98.237116</v>
+      </c>
+      <c r="C197">
+        <v>16.25</v>
+      </c>
+      <c r="D197">
+        <v>174.18</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>98.237116</v>
+      </c>
+      <c r="B198">
+        <v>98.361024999999998</v>
+      </c>
+      <c r="C198">
+        <v>16.332999999999998</v>
+      </c>
+      <c r="D198">
+        <v>174.42</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>98.361024999999998</v>
+      </c>
+      <c r="B199">
+        <v>98.484933999999996</v>
+      </c>
+      <c r="C199">
+        <v>16.417000000000002</v>
+      </c>
+      <c r="D199">
+        <v>174.64</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>98.484933999999996</v>
+      </c>
+      <c r="B200">
+        <v>98.597577999999999</v>
+      </c>
+      <c r="C200">
+        <v>16.5</v>
+      </c>
+      <c r="D200">
+        <v>174.86</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>98.597577999999999</v>
+      </c>
+      <c r="B201">
+        <v>98.704589999999996</v>
+      </c>
+      <c r="C201">
+        <v>16.582999999999998</v>
+      </c>
+      <c r="D201">
+        <v>175.06</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>98.704589999999996</v>
+      </c>
+      <c r="B202">
+        <v>98.805970000000002</v>
+      </c>
+      <c r="C202">
+        <v>16.667000000000002</v>
+      </c>
+      <c r="D202">
+        <v>175.25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>98.805970000000002</v>
+      </c>
+      <c r="B203">
+        <v>98.907349999999994</v>
+      </c>
+      <c r="C203">
+        <v>16.75</v>
+      </c>
+      <c r="D203">
+        <v>175.43</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>98.907349999999994</v>
+      </c>
+      <c r="B204">
+        <v>98.997466000000003</v>
+      </c>
+      <c r="C204">
+        <v>16.832999999999998</v>
+      </c>
+      <c r="D204">
+        <v>175.61</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>98.997466000000003</v>
+      </c>
+      <c r="B205">
+        <v>99.081948999999994</v>
+      </c>
+      <c r="C205">
+        <v>16.917000000000002</v>
+      </c>
+      <c r="D205">
+        <v>175.77</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>99.081948999999994</v>
+      </c>
+      <c r="B206">
+        <v>99.166432</v>
+      </c>
+      <c r="C206">
+        <v>17</v>
+      </c>
+      <c r="D206">
+        <v>175.92</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>99.166432</v>
+      </c>
+      <c r="B207">
+        <v>99.245283000000001</v>
+      </c>
+      <c r="C207">
+        <v>17.082999999999998</v>
+      </c>
+      <c r="D207">
+        <v>176.07</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>99.245283000000001</v>
+      </c>
+      <c r="B208">
+        <v>99.312870000000004</v>
+      </c>
+      <c r="C208">
+        <v>17.167000000000002</v>
+      </c>
+      <c r="D208">
+        <v>176.21</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>99.312870000000004</v>
+      </c>
+      <c r="B209">
+        <v>99.380455999999995</v>
+      </c>
+      <c r="C209">
+        <v>17.25</v>
+      </c>
+      <c r="D209">
+        <v>176.33</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>99.380455999999995</v>
+      </c>
+      <c r="B210">
+        <v>99.448042999999998</v>
+      </c>
+      <c r="C210">
+        <v>17.332999999999998</v>
+      </c>
+      <c r="D210">
+        <v>176.45</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>99.448042999999998</v>
+      </c>
+      <c r="B211">
+        <v>99.504365000000007</v>
+      </c>
+      <c r="C211">
+        <v>17.417000000000002</v>
+      </c>
+      <c r="D211">
+        <v>176.57</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>99.504365000000007</v>
+      </c>
+      <c r="B212">
+        <v>99.555054999999996</v>
+      </c>
+      <c r="C212">
+        <v>17.5</v>
+      </c>
+      <c r="D212">
+        <v>176.67</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>99.555054999999996</v>
+      </c>
+      <c r="B213">
+        <v>99.605744999999999</v>
+      </c>
+      <c r="C213">
+        <v>17.582999999999998</v>
+      </c>
+      <c r="D213">
+        <v>176.76</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>99.605744999999999</v>
+      </c>
+      <c r="B214">
+        <v>99.645169999999993</v>
+      </c>
+      <c r="C214">
+        <v>17.667000000000002</v>
+      </c>
+      <c r="D214">
+        <v>176.85</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>99.645169999999993</v>
+      </c>
+      <c r="B215">
+        <v>99.684595999999999</v>
+      </c>
+      <c r="C215">
+        <v>17.75</v>
+      </c>
+      <c r="D215">
+        <v>176.92</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>99.684595999999999</v>
+      </c>
+      <c r="B216">
+        <v>99.712756999999996</v>
+      </c>
+      <c r="C216">
+        <v>17.832999999999998</v>
+      </c>
+      <c r="D216">
+        <v>176.99</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>99.712756999999996</v>
+      </c>
+      <c r="B217">
+        <v>99.740917999999994</v>
+      </c>
+      <c r="C217">
+        <v>17.917000000000002</v>
+      </c>
+      <c r="D217">
+        <v>177.04</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>99.740917999999994</v>
+      </c>
+      <c r="B218">
+        <v>0</v>
+      </c>
+      <c r="C218">
+        <v>18</v>
+      </c>
+      <c r="D218">
+        <v>177.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Turkish, Norwegian, and Belgian growth references
</commit_message>
<xml_diff>
--- a/data-raw/maturation.xlsx
+++ b/data-raw/maturation.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdukikhia/Documents/R Packages/ageR/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04F370-A91D-F642-A7A7-E5200F86C3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9F0789-BFD6-3A46-8026-3F6BC3452C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17640" activeTab="5" xr2:uid="{1F346313-5E37-0D4E-9152-608513635295}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17640" firstSheet="3" activeTab="4" xr2:uid="{1F346313-5E37-0D4E-9152-608513635295}"/>
   </bookViews>
   <sheets>
     <sheet name="maturation" sheetId="1" r:id="rId1"/>
     <sheet name="table" sheetId="2" r:id="rId2"/>
     <sheet name="CDC curves" sheetId="3" r:id="rId3"/>
     <sheet name="UK90 curves" sheetId="4" r:id="rId4"/>
-    <sheet name="Zscores" sheetId="5" r:id="rId5"/>
-    <sheet name="Bio Age" sheetId="6" r:id="rId6"/>
+    <sheet name="Turkey curves" sheetId="7" r:id="rId5"/>
+    <sheet name="Belgium curves" sheetId="8" r:id="rId6"/>
+    <sheet name="Norway curves" sheetId="9" r:id="rId7"/>
+    <sheet name="Zscores" sheetId="5" r:id="rId8"/>
+    <sheet name="Bio Age" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="75">
   <si>
     <t>Player Name</t>
   </si>
@@ -344,9 +347,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -384,7 +387,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -490,7 +493,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -632,7 +635,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2668,7 +2671,7 @@
   <dimension ref="A1:N315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16542,8 +16545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509422DF-31AA-0541-89F7-F5887C8856E2}">
   <dimension ref="A1:N315"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30414,6 +30417,3349 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663AEFDD-DDAA-8041-9F82-E055935A8F4C}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>121.5</v>
+      </c>
+      <c r="E2">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F2">
+        <v>112.1</v>
+      </c>
+      <c r="G2">
+        <v>113.6</v>
+      </c>
+      <c r="H2">
+        <v>115.1</v>
+      </c>
+      <c r="I2">
+        <v>118.2</v>
+      </c>
+      <c r="J2">
+        <v>121.5</v>
+      </c>
+      <c r="K2">
+        <v>124.9</v>
+      </c>
+      <c r="L2">
+        <v>128</v>
+      </c>
+      <c r="M2">
+        <v>130</v>
+      </c>
+      <c r="N2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>126.9</v>
+      </c>
+      <c r="E3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F3">
+        <v>116.9</v>
+      </c>
+      <c r="G3">
+        <v>118.4</v>
+      </c>
+      <c r="H3">
+        <v>120</v>
+      </c>
+      <c r="I3">
+        <v>123.3</v>
+      </c>
+      <c r="J3">
+        <v>126.9</v>
+      </c>
+      <c r="K3">
+        <v>130.5</v>
+      </c>
+      <c r="L3">
+        <v>133.69999999999999</v>
+      </c>
+      <c r="M3">
+        <v>136</v>
+      </c>
+      <c r="N3">
+        <v>136.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>132.1</v>
+      </c>
+      <c r="E4">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F4">
+        <v>121.6</v>
+      </c>
+      <c r="G4">
+        <v>123.3</v>
+      </c>
+      <c r="H4">
+        <v>124.9</v>
+      </c>
+      <c r="I4">
+        <v>128.30000000000001</v>
+      </c>
+      <c r="J4">
+        <v>132.1</v>
+      </c>
+      <c r="K4">
+        <v>135.9</v>
+      </c>
+      <c r="L4">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="M4">
+        <v>141.5</v>
+      </c>
+      <c r="N4">
+        <v>142.69999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>137.6</v>
+      </c>
+      <c r="E5">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <v>126.4</v>
+      </c>
+      <c r="G5">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="H5">
+        <v>130</v>
+      </c>
+      <c r="I5">
+        <v>133.6</v>
+      </c>
+      <c r="J5">
+        <v>137.6</v>
+      </c>
+      <c r="K5">
+        <v>141.6</v>
+      </c>
+      <c r="L5">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="M5">
+        <v>147.69999999999999</v>
+      </c>
+      <c r="N5">
+        <v>148.69999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>143.80000000000001</v>
+      </c>
+      <c r="E6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>131.69999999999999</v>
+      </c>
+      <c r="G6">
+        <v>133.5</v>
+      </c>
+      <c r="H6">
+        <v>135.5</v>
+      </c>
+      <c r="I6">
+        <v>139.4</v>
+      </c>
+      <c r="J6">
+        <v>143.80000000000001</v>
+      </c>
+      <c r="K6">
+        <v>148.1</v>
+      </c>
+      <c r="L6">
+        <v>152</v>
+      </c>
+      <c r="M6">
+        <v>154.80000000000001</v>
+      </c>
+      <c r="N6">
+        <v>155.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>150.6</v>
+      </c>
+      <c r="E7">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F7">
+        <v>137</v>
+      </c>
+      <c r="G7">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="H7">
+        <v>141.30000000000001</v>
+      </c>
+      <c r="I7">
+        <v>145.69999999999999</v>
+      </c>
+      <c r="J7">
+        <v>150.6</v>
+      </c>
+      <c r="K7">
+        <v>155.4</v>
+      </c>
+      <c r="L7">
+        <v>159.80000000000001</v>
+      </c>
+      <c r="M7">
+        <v>163</v>
+      </c>
+      <c r="N7">
+        <v>164.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>157.69999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>142.80000000000001</v>
+      </c>
+      <c r="G8">
+        <v>145.19999999999999</v>
+      </c>
+      <c r="H8">
+        <v>147.6</v>
+      </c>
+      <c r="I8">
+        <v>152.4</v>
+      </c>
+      <c r="J8">
+        <v>157.69999999999999</v>
+      </c>
+      <c r="K8">
+        <v>163.1</v>
+      </c>
+      <c r="L8">
+        <v>167.9</v>
+      </c>
+      <c r="M8">
+        <v>171.2</v>
+      </c>
+      <c r="N8">
+        <v>172.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>164.9</v>
+      </c>
+      <c r="E9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F9">
+        <v>150.30000000000001</v>
+      </c>
+      <c r="G9">
+        <v>152.6</v>
+      </c>
+      <c r="H9">
+        <v>155</v>
+      </c>
+      <c r="I9">
+        <v>159.69999999999999</v>
+      </c>
+      <c r="J9">
+        <v>164.9</v>
+      </c>
+      <c r="K9">
+        <v>170.1</v>
+      </c>
+      <c r="L9">
+        <v>174.8</v>
+      </c>
+      <c r="M9">
+        <v>178.2</v>
+      </c>
+      <c r="N9">
+        <v>179.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>170.3</v>
+      </c>
+      <c r="E10">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F10">
+        <v>156.9</v>
+      </c>
+      <c r="G10">
+        <v>158.9</v>
+      </c>
+      <c r="H10">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="I10">
+        <v>165.5</v>
+      </c>
+      <c r="J10">
+        <v>170.3</v>
+      </c>
+      <c r="K10">
+        <v>175.1</v>
+      </c>
+      <c r="L10">
+        <v>179.4</v>
+      </c>
+      <c r="M10">
+        <v>182.5</v>
+      </c>
+      <c r="N10">
+        <v>183.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>173.4</v>
+      </c>
+      <c r="E11">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <v>160.9</v>
+      </c>
+      <c r="G11">
+        <v>162.9</v>
+      </c>
+      <c r="H11">
+        <v>164.9</v>
+      </c>
+      <c r="I11">
+        <v>168.9</v>
+      </c>
+      <c r="J11">
+        <v>173.4</v>
+      </c>
+      <c r="K11">
+        <v>177.9</v>
+      </c>
+      <c r="L11">
+        <v>181.9</v>
+      </c>
+      <c r="M11">
+        <v>184.6</v>
+      </c>
+      <c r="N11">
+        <v>185.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>175</v>
+      </c>
+      <c r="E12">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F12">
+        <v>163</v>
+      </c>
+      <c r="G12">
+        <v>164.7</v>
+      </c>
+      <c r="H12">
+        <v>166.8</v>
+      </c>
+      <c r="I12">
+        <v>170.7</v>
+      </c>
+      <c r="J12">
+        <v>175</v>
+      </c>
+      <c r="K12">
+        <v>179.3</v>
+      </c>
+      <c r="L12">
+        <v>183.2</v>
+      </c>
+      <c r="M12">
+        <v>186</v>
+      </c>
+      <c r="N12">
+        <v>187.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>176.2</v>
+      </c>
+      <c r="E13">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F13">
+        <v>164.5</v>
+      </c>
+      <c r="G13">
+        <v>166.3</v>
+      </c>
+      <c r="H13">
+        <v>168.2</v>
+      </c>
+      <c r="I13">
+        <v>172</v>
+      </c>
+      <c r="J13">
+        <v>176.2</v>
+      </c>
+      <c r="K13">
+        <v>180.4</v>
+      </c>
+      <c r="L13">
+        <v>184.2</v>
+      </c>
+      <c r="M13">
+        <v>186.6</v>
+      </c>
+      <c r="N13">
+        <v>187.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>121.1</v>
+      </c>
+      <c r="E14">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F14">
+        <v>111.6</v>
+      </c>
+      <c r="G14">
+        <v>113.2</v>
+      </c>
+      <c r="H14">
+        <v>114.6</v>
+      </c>
+      <c r="I14">
+        <v>117.7</v>
+      </c>
+      <c r="J14">
+        <v>121.1</v>
+      </c>
+      <c r="K14">
+        <v>124.4</v>
+      </c>
+      <c r="L14">
+        <v>127.5</v>
+      </c>
+      <c r="M14">
+        <v>129.5</v>
+      </c>
+      <c r="N14">
+        <v>130.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>126.7</v>
+      </c>
+      <c r="E15">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F15">
+        <v>116.7</v>
+      </c>
+      <c r="G15">
+        <v>118.2</v>
+      </c>
+      <c r="H15">
+        <v>119.9</v>
+      </c>
+      <c r="I15">
+        <v>123.1</v>
+      </c>
+      <c r="J15">
+        <v>126.7</v>
+      </c>
+      <c r="K15">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="L15">
+        <v>133.5</v>
+      </c>
+      <c r="M15">
+        <v>135.80000000000001</v>
+      </c>
+      <c r="N15">
+        <v>136.69999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>132.1</v>
+      </c>
+      <c r="E16">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F16">
+        <v>121.3</v>
+      </c>
+      <c r="G16">
+        <v>122.9</v>
+      </c>
+      <c r="H16">
+        <v>124.7</v>
+      </c>
+      <c r="I16">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="J16">
+        <v>132.1</v>
+      </c>
+      <c r="K16">
+        <v>136</v>
+      </c>
+      <c r="L16">
+        <v>139.5</v>
+      </c>
+      <c r="M16">
+        <v>142</v>
+      </c>
+      <c r="N16">
+        <v>142.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>137.9</v>
+      </c>
+      <c r="E17">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F17">
+        <v>125.8</v>
+      </c>
+      <c r="G17">
+        <v>127.6</v>
+      </c>
+      <c r="H17">
+        <v>129.6</v>
+      </c>
+      <c r="I17">
+        <v>133.5</v>
+      </c>
+      <c r="J17">
+        <v>137.9</v>
+      </c>
+      <c r="K17">
+        <v>142.19999999999999</v>
+      </c>
+      <c r="L17">
+        <v>146.1</v>
+      </c>
+      <c r="M17">
+        <v>149</v>
+      </c>
+      <c r="N17">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>145.4</v>
+      </c>
+      <c r="E18">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F18">
+        <v>132.5</v>
+      </c>
+      <c r="G18">
+        <v>134.6</v>
+      </c>
+      <c r="H18">
+        <v>136.6</v>
+      </c>
+      <c r="I18">
+        <v>140.80000000000001</v>
+      </c>
+      <c r="J18">
+        <v>145.4</v>
+      </c>
+      <c r="K18">
+        <v>150.1</v>
+      </c>
+      <c r="L18">
+        <v>154.19999999999999</v>
+      </c>
+      <c r="M18">
+        <v>157.1</v>
+      </c>
+      <c r="N18">
+        <v>158.30000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>153.1</v>
+      </c>
+      <c r="E19">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F19">
+        <v>141.1</v>
+      </c>
+      <c r="G19">
+        <v>142.9</v>
+      </c>
+      <c r="H19">
+        <v>144.9</v>
+      </c>
+      <c r="I19">
+        <v>148.80000000000001</v>
+      </c>
+      <c r="J19">
+        <v>153.1</v>
+      </c>
+      <c r="K19">
+        <v>157.4</v>
+      </c>
+      <c r="L19">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="M19">
+        <v>164.1</v>
+      </c>
+      <c r="N19">
+        <v>165.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="E20">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F20">
+        <v>146.6</v>
+      </c>
+      <c r="G20">
+        <v>148.19999999999999</v>
+      </c>
+      <c r="H20">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="I20">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="J20">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="K20">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="L20">
+        <v>165.5</v>
+      </c>
+      <c r="M20">
+        <v>168</v>
+      </c>
+      <c r="N20">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>260.39999999999998</v>
+      </c>
+      <c r="E21">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F21">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="G21">
+        <v>245</v>
+      </c>
+      <c r="H21">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="I21">
+        <v>156.4</v>
+      </c>
+      <c r="J21">
+        <v>260.39999999999998</v>
+      </c>
+      <c r="K21">
+        <v>164.3</v>
+      </c>
+      <c r="L21">
+        <v>169.3</v>
+      </c>
+      <c r="M21">
+        <v>276.7</v>
+      </c>
+      <c r="N21">
+        <v>171.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>161.69999999999999</v>
+      </c>
+      <c r="E22">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F22">
+        <v>150.69999999999999</v>
+      </c>
+      <c r="G22">
+        <v>152.4</v>
+      </c>
+      <c r="H22">
+        <v>154.19999999999999</v>
+      </c>
+      <c r="I22">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="J22">
+        <v>161.69999999999999</v>
+      </c>
+      <c r="K22">
+        <v>165.7</v>
+      </c>
+      <c r="L22">
+        <v>169.3</v>
+      </c>
+      <c r="M22">
+        <v>171.6</v>
+      </c>
+      <c r="N22">
+        <v>172.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>162.4</v>
+      </c>
+      <c r="E23">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F23">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="G23">
+        <v>153.1</v>
+      </c>
+      <c r="H23">
+        <v>154.80000000000001</v>
+      </c>
+      <c r="I23">
+        <v>158.4</v>
+      </c>
+      <c r="J23">
+        <v>162.4</v>
+      </c>
+      <c r="K23">
+        <v>166.3</v>
+      </c>
+      <c r="L23">
+        <v>169.9</v>
+      </c>
+      <c r="M23">
+        <v>172.3</v>
+      </c>
+      <c r="N23">
+        <v>173.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="E24">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F24">
+        <v>151.69999999999999</v>
+      </c>
+      <c r="G24">
+        <v>153.30000000000001</v>
+      </c>
+      <c r="H24">
+        <v>155.19999999999999</v>
+      </c>
+      <c r="I24">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="J24">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="K24">
+        <v>166.7</v>
+      </c>
+      <c r="L24">
+        <v>170.3</v>
+      </c>
+      <c r="M24">
+        <v>172.6</v>
+      </c>
+      <c r="N24">
+        <v>173.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>163.1</v>
+      </c>
+      <c r="E25">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F25">
+        <v>152</v>
+      </c>
+      <c r="G25">
+        <v>153.69999999999999</v>
+      </c>
+      <c r="H25">
+        <v>155.6</v>
+      </c>
+      <c r="I25">
+        <v>159.1</v>
+      </c>
+      <c r="J25">
+        <v>163.1</v>
+      </c>
+      <c r="K25">
+        <v>167.1</v>
+      </c>
+      <c r="L25">
+        <v>170.7</v>
+      </c>
+      <c r="M25">
+        <v>173</v>
+      </c>
+      <c r="N25">
+        <v>174.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B621282F-4F3F-1E46-9D17-20CBB6F27887}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>123.8</v>
+      </c>
+      <c r="E2">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F2">
+        <v>114.4</v>
+      </c>
+      <c r="G2">
+        <v>115.5</v>
+      </c>
+      <c r="H2">
+        <v>117.3</v>
+      </c>
+      <c r="I2">
+        <v>120.3</v>
+      </c>
+      <c r="J2">
+        <v>123.8</v>
+      </c>
+      <c r="K2">
+        <v>127.4</v>
+      </c>
+      <c r="L2">
+        <v>130.6</v>
+      </c>
+      <c r="M2">
+        <v>132.69999999999999</v>
+      </c>
+      <c r="N2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>129.9</v>
+      </c>
+      <c r="E3">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F3">
+        <v>120</v>
+      </c>
+      <c r="G3">
+        <v>121.2</v>
+      </c>
+      <c r="H3">
+        <v>123.1</v>
+      </c>
+      <c r="I3">
+        <v>126.3</v>
+      </c>
+      <c r="J3">
+        <v>129.9</v>
+      </c>
+      <c r="K3">
+        <v>133.6</v>
+      </c>
+      <c r="L3">
+        <v>137.1</v>
+      </c>
+      <c r="M3">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="N3">
+        <v>140.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>135.4</v>
+      </c>
+      <c r="E4">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F4">
+        <v>124.9</v>
+      </c>
+      <c r="G4">
+        <v>126.2</v>
+      </c>
+      <c r="H4">
+        <v>128.1</v>
+      </c>
+      <c r="I4">
+        <v>131.5</v>
+      </c>
+      <c r="J4">
+        <v>135.4</v>
+      </c>
+      <c r="K4">
+        <v>139.4</v>
+      </c>
+      <c r="L4">
+        <v>143.1</v>
+      </c>
+      <c r="M4">
+        <v>145.30000000000001</v>
+      </c>
+      <c r="N4">
+        <v>146.80000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>140.5</v>
+      </c>
+      <c r="E5">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <v>129.6</v>
+      </c>
+      <c r="G5">
+        <v>130.9</v>
+      </c>
+      <c r="H5">
+        <v>133</v>
+      </c>
+      <c r="I5">
+        <v>136.5</v>
+      </c>
+      <c r="J5">
+        <v>140.5</v>
+      </c>
+      <c r="K5">
+        <v>144.6</v>
+      </c>
+      <c r="L5">
+        <v>148.5</v>
+      </c>
+      <c r="M5">
+        <v>150.80000000000001</v>
+      </c>
+      <c r="N5">
+        <v>152.30000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="E6">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F6">
+        <v>134.19999999999999</v>
+      </c>
+      <c r="G6">
+        <v>135.6</v>
+      </c>
+      <c r="H6">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="I6">
+        <v>141.5</v>
+      </c>
+      <c r="J6">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="K6">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="L6">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="M6">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="N6">
+        <v>158.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>152</v>
+      </c>
+      <c r="E7">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>139.4</v>
+      </c>
+      <c r="G7">
+        <v>140.9</v>
+      </c>
+      <c r="H7">
+        <v>143.30000000000001</v>
+      </c>
+      <c r="I7">
+        <v>147.4</v>
+      </c>
+      <c r="J7">
+        <v>152</v>
+      </c>
+      <c r="K7">
+        <v>156.80000000000001</v>
+      </c>
+      <c r="L7">
+        <v>161.19999999999999</v>
+      </c>
+      <c r="M7">
+        <v>163.9</v>
+      </c>
+      <c r="N7">
+        <v>165.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="E8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>145.1</v>
+      </c>
+      <c r="G8">
+        <v>146.69999999999999</v>
+      </c>
+      <c r="H8">
+        <v>149.30000000000001</v>
+      </c>
+      <c r="I8">
+        <v>153.69999999999999</v>
+      </c>
+      <c r="J8">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="K8">
+        <v>164</v>
+      </c>
+      <c r="L8">
+        <v>168.9</v>
+      </c>
+      <c r="M8">
+        <v>171.8</v>
+      </c>
+      <c r="N8">
+        <v>173.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>166</v>
+      </c>
+      <c r="E9">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F9">
+        <v>152</v>
+      </c>
+      <c r="G9">
+        <v>153.69999999999999</v>
+      </c>
+      <c r="H9">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="I9">
+        <v>160.80000000000001</v>
+      </c>
+      <c r="J9">
+        <v>166</v>
+      </c>
+      <c r="K9">
+        <v>171.3</v>
+      </c>
+      <c r="L9">
+        <v>176.3</v>
+      </c>
+      <c r="M9">
+        <v>179.3</v>
+      </c>
+      <c r="N9">
+        <v>181.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>171.9</v>
+      </c>
+      <c r="E10">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F10">
+        <v>158.19999999999999</v>
+      </c>
+      <c r="G10">
+        <v>159.9</v>
+      </c>
+      <c r="H10">
+        <v>162.5</v>
+      </c>
+      <c r="I10">
+        <v>166.9</v>
+      </c>
+      <c r="J10">
+        <v>171.9</v>
+      </c>
+      <c r="K10">
+        <v>177.1</v>
+      </c>
+      <c r="L10">
+        <v>181.9</v>
+      </c>
+      <c r="M10">
+        <v>184.8</v>
+      </c>
+      <c r="N10">
+        <v>186.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>175.8</v>
+      </c>
+      <c r="E11">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F11">
+        <v>162.80000000000001</v>
+      </c>
+      <c r="G11">
+        <v>164.3</v>
+      </c>
+      <c r="H11">
+        <v>166.8</v>
+      </c>
+      <c r="I11">
+        <v>171</v>
+      </c>
+      <c r="J11">
+        <v>175.8</v>
+      </c>
+      <c r="K11">
+        <v>180.7</v>
+      </c>
+      <c r="L11">
+        <v>185.3</v>
+      </c>
+      <c r="M11">
+        <v>188.1</v>
+      </c>
+      <c r="N11">
+        <v>189.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>178.1</v>
+      </c>
+      <c r="E12">
+        <v>3.9E-2</v>
+      </c>
+      <c r="F12">
+        <v>165.5</v>
+      </c>
+      <c r="G12">
+        <v>167</v>
+      </c>
+      <c r="H12">
+        <v>169.4</v>
+      </c>
+      <c r="I12">
+        <v>173.5</v>
+      </c>
+      <c r="J12">
+        <v>178.1</v>
+      </c>
+      <c r="K12">
+        <v>182.8</v>
+      </c>
+      <c r="L12">
+        <v>187.2</v>
+      </c>
+      <c r="M12">
+        <v>189.9</v>
+      </c>
+      <c r="N12">
+        <v>191.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>179.4</v>
+      </c>
+      <c r="E13">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>167</v>
+      </c>
+      <c r="G13">
+        <v>168.5</v>
+      </c>
+      <c r="H13">
+        <v>170.9</v>
+      </c>
+      <c r="I13">
+        <v>174.9</v>
+      </c>
+      <c r="J13">
+        <v>179.4</v>
+      </c>
+      <c r="K13">
+        <v>184.1</v>
+      </c>
+      <c r="L13">
+        <v>188.4</v>
+      </c>
+      <c r="M13">
+        <v>191</v>
+      </c>
+      <c r="N13">
+        <v>192.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>123</v>
+      </c>
+      <c r="E14">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F14">
+        <v>113.4</v>
+      </c>
+      <c r="G14">
+        <v>114.6</v>
+      </c>
+      <c r="H14">
+        <v>116.4</v>
+      </c>
+      <c r="I14">
+        <v>119.5</v>
+      </c>
+      <c r="J14">
+        <v>123</v>
+      </c>
+      <c r="K14">
+        <v>126.6</v>
+      </c>
+      <c r="L14">
+        <v>130</v>
+      </c>
+      <c r="M14">
+        <v>132</v>
+      </c>
+      <c r="N14">
+        <v>133.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>129</v>
+      </c>
+      <c r="E15">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F15">
+        <v>118.8</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+      <c r="H15">
+        <v>121.9</v>
+      </c>
+      <c r="I15">
+        <v>125.2</v>
+      </c>
+      <c r="J15">
+        <v>129</v>
+      </c>
+      <c r="K15">
+        <v>132.9</v>
+      </c>
+      <c r="L15">
+        <v>136.5</v>
+      </c>
+      <c r="M15">
+        <v>138.69999999999999</v>
+      </c>
+      <c r="N15">
+        <v>140.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>134.30000000000001</v>
+      </c>
+      <c r="E16">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F16">
+        <v>123.6</v>
+      </c>
+      <c r="G16">
+        <v>124.9</v>
+      </c>
+      <c r="H16">
+        <v>126.9</v>
+      </c>
+      <c r="I16">
+        <v>130.4</v>
+      </c>
+      <c r="J16">
+        <v>134.30000000000001</v>
+      </c>
+      <c r="K16">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="L16">
+        <v>142.1</v>
+      </c>
+      <c r="M16">
+        <v>144.4</v>
+      </c>
+      <c r="N16">
+        <v>145.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>139.9</v>
+      </c>
+      <c r="E17">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F17">
+        <v>128.30000000000001</v>
+      </c>
+      <c r="G17">
+        <v>129.69999999999999</v>
+      </c>
+      <c r="H17">
+        <v>131.9</v>
+      </c>
+      <c r="I17">
+        <v>135.6</v>
+      </c>
+      <c r="J17">
+        <v>139.9</v>
+      </c>
+      <c r="K17">
+        <v>144.30000000000001</v>
+      </c>
+      <c r="L17">
+        <v>148.4</v>
+      </c>
+      <c r="M17">
+        <v>150.9</v>
+      </c>
+      <c r="N17">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>146.6</v>
+      </c>
+      <c r="E18">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F18">
+        <v>134.19999999999999</v>
+      </c>
+      <c r="G18">
+        <v>135.69999999999999</v>
+      </c>
+      <c r="H18">
+        <v>138</v>
+      </c>
+      <c r="I18">
+        <v>142</v>
+      </c>
+      <c r="J18">
+        <v>146.6</v>
+      </c>
+      <c r="K18">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="L18">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="M18">
+        <v>158.4</v>
+      </c>
+      <c r="N18">
+        <v>160.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>153.19999999999999</v>
+      </c>
+      <c r="E19">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>140.5</v>
+      </c>
+      <c r="G19">
+        <v>142</v>
+      </c>
+      <c r="H19">
+        <v>144.4</v>
+      </c>
+      <c r="I19">
+        <v>148.5</v>
+      </c>
+      <c r="J19">
+        <v>153.19999999999999</v>
+      </c>
+      <c r="K19">
+        <v>158</v>
+      </c>
+      <c r="L19">
+        <v>162.5</v>
+      </c>
+      <c r="M19">
+        <v>165.2</v>
+      </c>
+      <c r="N19">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>158.69999999999999</v>
+      </c>
+      <c r="E20">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F20">
+        <v>146.4</v>
+      </c>
+      <c r="G20">
+        <v>147.9</v>
+      </c>
+      <c r="H20">
+        <v>150.19999999999999</v>
+      </c>
+      <c r="I20">
+        <v>154.19999999999999</v>
+      </c>
+      <c r="J20">
+        <v>158.69999999999999</v>
+      </c>
+      <c r="K20">
+        <v>163.4</v>
+      </c>
+      <c r="L20">
+        <v>167.7</v>
+      </c>
+      <c r="M20">
+        <v>170.3</v>
+      </c>
+      <c r="N20">
+        <v>172.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>162.4</v>
+      </c>
+      <c r="E21">
+        <v>0.04</v>
+      </c>
+      <c r="F21">
+        <v>150.6</v>
+      </c>
+      <c r="G21">
+        <v>152.1</v>
+      </c>
+      <c r="H21">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="I21">
+        <v>158.1</v>
+      </c>
+      <c r="J21">
+        <v>162.4</v>
+      </c>
+      <c r="K21">
+        <v>166.8</v>
+      </c>
+      <c r="L21">
+        <v>170.9</v>
+      </c>
+      <c r="M21">
+        <v>173.4</v>
+      </c>
+      <c r="N21">
+        <v>175.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>164.7</v>
+      </c>
+      <c r="E22">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F22">
+        <v>153.30000000000001</v>
+      </c>
+      <c r="G22">
+        <v>154.69999999999999</v>
+      </c>
+      <c r="H22">
+        <v>156.9</v>
+      </c>
+      <c r="I22">
+        <v>160.5</v>
+      </c>
+      <c r="J22">
+        <v>164.7</v>
+      </c>
+      <c r="K22">
+        <v>169</v>
+      </c>
+      <c r="L22">
+        <v>172.9</v>
+      </c>
+      <c r="M22">
+        <v>175.3</v>
+      </c>
+      <c r="N22">
+        <v>176.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>165.8</v>
+      </c>
+      <c r="E23">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F23">
+        <v>154.9</v>
+      </c>
+      <c r="G23">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="H23">
+        <v>158.30000000000001</v>
+      </c>
+      <c r="I23">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="J23">
+        <v>165.8</v>
+      </c>
+      <c r="K23">
+        <v>169.9</v>
+      </c>
+      <c r="L23">
+        <v>173.6</v>
+      </c>
+      <c r="M23">
+        <v>175.9</v>
+      </c>
+      <c r="N23">
+        <v>177.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>166.2</v>
+      </c>
+      <c r="E24">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F24">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="G24">
+        <v>156.6</v>
+      </c>
+      <c r="H24">
+        <v>158.69999999999999</v>
+      </c>
+      <c r="I24">
+        <v>162.19999999999999</v>
+      </c>
+      <c r="J24">
+        <v>166.2</v>
+      </c>
+      <c r="K24">
+        <v>170.3</v>
+      </c>
+      <c r="L24">
+        <v>174</v>
+      </c>
+      <c r="M24">
+        <v>176.3</v>
+      </c>
+      <c r="N24">
+        <v>177.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>166.3</v>
+      </c>
+      <c r="E25">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F25">
+        <v>155.4</v>
+      </c>
+      <c r="G25">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="H25">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I25">
+        <v>162.30000000000001</v>
+      </c>
+      <c r="J25">
+        <v>166.3</v>
+      </c>
+      <c r="K25">
+        <v>170.4</v>
+      </c>
+      <c r="L25">
+        <v>174.2</v>
+      </c>
+      <c r="M25">
+        <v>176.4</v>
+      </c>
+      <c r="N25">
+        <v>177.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEEADE3-FC3F-9840-9458-6D9E58369C21}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>124.6</v>
+      </c>
+      <c r="E2">
+        <v>4.07E-2</v>
+      </c>
+      <c r="F2">
+        <v>115.4</v>
+      </c>
+      <c r="G2">
+        <v>116.5</v>
+      </c>
+      <c r="H2">
+        <v>118.3</v>
+      </c>
+      <c r="I2">
+        <v>121.2</v>
+      </c>
+      <c r="J2">
+        <v>124.6</v>
+      </c>
+      <c r="K2">
+        <v>128.1</v>
+      </c>
+      <c r="L2">
+        <v>131.30000000000001</v>
+      </c>
+      <c r="M2">
+        <v>133.19999999999999</v>
+      </c>
+      <c r="N2">
+        <v>134.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="E3">
+        <v>4.1500000000000002E-2</v>
+      </c>
+      <c r="F3">
+        <v>121</v>
+      </c>
+      <c r="G3">
+        <v>122.2</v>
+      </c>
+      <c r="H3">
+        <v>124</v>
+      </c>
+      <c r="I3">
+        <v>127.2</v>
+      </c>
+      <c r="J3">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="K3">
+        <v>134.5</v>
+      </c>
+      <c r="L3">
+        <v>137.9</v>
+      </c>
+      <c r="M3">
+        <v>140</v>
+      </c>
+      <c r="N3">
+        <v>141.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>136.30000000000001</v>
+      </c>
+      <c r="E4">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="F4">
+        <v>125.9</v>
+      </c>
+      <c r="G4">
+        <v>127.1</v>
+      </c>
+      <c r="H4">
+        <v>129.1</v>
+      </c>
+      <c r="I4">
+        <v>132.5</v>
+      </c>
+      <c r="J4">
+        <v>136.30000000000001</v>
+      </c>
+      <c r="K4">
+        <v>140.19999999999999</v>
+      </c>
+      <c r="L4">
+        <v>143.9</v>
+      </c>
+      <c r="M4">
+        <v>146.1</v>
+      </c>
+      <c r="N4">
+        <v>147.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>141.6</v>
+      </c>
+      <c r="E5">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <v>130.5</v>
+      </c>
+      <c r="G5">
+        <v>131.80000000000001</v>
+      </c>
+      <c r="H5">
+        <v>133.9</v>
+      </c>
+      <c r="I5">
+        <v>137.5</v>
+      </c>
+      <c r="J5">
+        <v>141.6</v>
+      </c>
+      <c r="K5">
+        <v>145.80000000000001</v>
+      </c>
+      <c r="L5">
+        <v>149.69999999999999</v>
+      </c>
+      <c r="M5">
+        <v>152.1</v>
+      </c>
+      <c r="N5">
+        <v>153.69999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>147</v>
+      </c>
+      <c r="E6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>135.1</v>
+      </c>
+      <c r="G6">
+        <v>136.5</v>
+      </c>
+      <c r="H6">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="I6">
+        <v>142.6</v>
+      </c>
+      <c r="J6">
+        <v>147</v>
+      </c>
+      <c r="K6">
+        <v>151.5</v>
+      </c>
+      <c r="L6">
+        <v>155.69999999999999</v>
+      </c>
+      <c r="M6">
+        <v>158.30000000000001</v>
+      </c>
+      <c r="N6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="E7">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="F7">
+        <v>140</v>
+      </c>
+      <c r="G7">
+        <v>141.5</v>
+      </c>
+      <c r="H7">
+        <v>143.9</v>
+      </c>
+      <c r="I7">
+        <v>148.1</v>
+      </c>
+      <c r="J7">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="K7">
+        <v>157.69999999999999</v>
+      </c>
+      <c r="L7">
+        <v>162.19999999999999</v>
+      </c>
+      <c r="M7">
+        <v>165</v>
+      </c>
+      <c r="N7">
+        <v>166.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>159.6</v>
+      </c>
+      <c r="E8">
+        <v>4.7800000000000002E-2</v>
+      </c>
+      <c r="F8">
+        <v>145.9</v>
+      </c>
+      <c r="G8">
+        <v>147.5</v>
+      </c>
+      <c r="H8">
+        <v>150.1</v>
+      </c>
+      <c r="I8">
+        <v>154.5</v>
+      </c>
+      <c r="J8">
+        <v>159.6</v>
+      </c>
+      <c r="K8">
+        <v>164.8</v>
+      </c>
+      <c r="L8">
+        <v>169.7</v>
+      </c>
+      <c r="M8">
+        <v>172.7</v>
+      </c>
+      <c r="N8">
+        <v>174.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>166.9</v>
+      </c>
+      <c r="E9">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="F9">
+        <v>152.80000000000001</v>
+      </c>
+      <c r="G9">
+        <v>154.5</v>
+      </c>
+      <c r="H9">
+        <v>157.19999999999999</v>
+      </c>
+      <c r="I9">
+        <v>161.69999999999999</v>
+      </c>
+      <c r="J9">
+        <v>166.9</v>
+      </c>
+      <c r="K9">
+        <v>172.3</v>
+      </c>
+      <c r="L9">
+        <v>177.2</v>
+      </c>
+      <c r="M9">
+        <v>180.3</v>
+      </c>
+      <c r="N9">
+        <v>182.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>173.2</v>
+      </c>
+      <c r="E10">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="F10">
+        <v>159.6</v>
+      </c>
+      <c r="G10">
+        <v>161.30000000000001</v>
+      </c>
+      <c r="H10">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="I10">
+        <v>168.2</v>
+      </c>
+      <c r="J10">
+        <v>173.2</v>
+      </c>
+      <c r="K10">
+        <v>178.3</v>
+      </c>
+      <c r="L10">
+        <v>183.1</v>
+      </c>
+      <c r="M10">
+        <v>186</v>
+      </c>
+      <c r="N10">
+        <v>187.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>177.5</v>
+      </c>
+      <c r="E11">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="F11">
+        <v>164.7</v>
+      </c>
+      <c r="G11">
+        <v>166.3</v>
+      </c>
+      <c r="H11">
+        <v>168.7</v>
+      </c>
+      <c r="I11">
+        <v>172.8</v>
+      </c>
+      <c r="J11">
+        <v>177.5</v>
+      </c>
+      <c r="K11">
+        <v>182.3</v>
+      </c>
+      <c r="L11">
+        <v>186.8</v>
+      </c>
+      <c r="M11">
+        <v>189.5</v>
+      </c>
+      <c r="N11">
+        <v>191.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>179.7</v>
+      </c>
+      <c r="E12">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>167.4</v>
+      </c>
+      <c r="G12">
+        <v>168.9</v>
+      </c>
+      <c r="H12">
+        <v>171.2</v>
+      </c>
+      <c r="I12">
+        <v>175.2</v>
+      </c>
+      <c r="J12">
+        <v>179.7</v>
+      </c>
+      <c r="K12">
+        <v>184.3</v>
+      </c>
+      <c r="L12">
+        <v>188.6</v>
+      </c>
+      <c r="M12">
+        <v>191.2</v>
+      </c>
+      <c r="N12">
+        <v>192.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>180.7</v>
+      </c>
+      <c r="E13">
+        <v>3.6700000000000003E-2</v>
+      </c>
+      <c r="F13">
+        <v>168.6</v>
+      </c>
+      <c r="G13">
+        <v>170.1</v>
+      </c>
+      <c r="H13">
+        <v>172.4</v>
+      </c>
+      <c r="I13">
+        <v>176.3</v>
+      </c>
+      <c r="J13">
+        <v>180.7</v>
+      </c>
+      <c r="K13">
+        <v>185.2</v>
+      </c>
+      <c r="L13">
+        <v>189.4</v>
+      </c>
+      <c r="M13">
+        <v>191.9</v>
+      </c>
+      <c r="N13">
+        <v>193.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>123.8</v>
+      </c>
+      <c r="E14">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="F14">
+        <v>114.3</v>
+      </c>
+      <c r="G14">
+        <v>115.5</v>
+      </c>
+      <c r="H14">
+        <v>117.3</v>
+      </c>
+      <c r="I14">
+        <v>120.3</v>
+      </c>
+      <c r="J14">
+        <v>123.8</v>
+      </c>
+      <c r="K14">
+        <v>127.4</v>
+      </c>
+      <c r="L14">
+        <v>130.69999999999999</v>
+      </c>
+      <c r="M14">
+        <v>132.69999999999999</v>
+      </c>
+      <c r="N14">
+        <v>134.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="E15">
+        <v>4.2900000000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>119.7</v>
+      </c>
+      <c r="G15">
+        <v>121</v>
+      </c>
+      <c r="H15">
+        <v>122.9</v>
+      </c>
+      <c r="I15">
+        <v>126.1</v>
+      </c>
+      <c r="J15">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="K15">
+        <v>133.6</v>
+      </c>
+      <c r="L15">
+        <v>137.1</v>
+      </c>
+      <c r="M15">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="N15">
+        <v>140.69999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>135</v>
+      </c>
+      <c r="E16">
+        <v>4.3299999999999998E-2</v>
+      </c>
+      <c r="F16">
+        <v>124.4</v>
+      </c>
+      <c r="G16">
+        <v>125.7</v>
+      </c>
+      <c r="H16">
+        <v>127.7</v>
+      </c>
+      <c r="I16">
+        <v>131.1</v>
+      </c>
+      <c r="J16">
+        <v>135</v>
+      </c>
+      <c r="K16">
+        <v>139</v>
+      </c>
+      <c r="L16">
+        <v>142.69999999999999</v>
+      </c>
+      <c r="M16">
+        <v>145</v>
+      </c>
+      <c r="N16">
+        <v>146.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>140.5</v>
+      </c>
+      <c r="E17">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F17">
+        <v>129.5</v>
+      </c>
+      <c r="G17">
+        <v>130.80000000000001</v>
+      </c>
+      <c r="H17">
+        <v>132.9</v>
+      </c>
+      <c r="I17">
+        <v>136.4</v>
+      </c>
+      <c r="J17">
+        <v>140.5</v>
+      </c>
+      <c r="K17">
+        <v>144.69999999999999</v>
+      </c>
+      <c r="L17">
+        <v>148.6</v>
+      </c>
+      <c r="M17">
+        <v>150.9</v>
+      </c>
+      <c r="N17">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>146.69999999999999</v>
+      </c>
+      <c r="E18">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="F18">
+        <v>135.30000000000001</v>
+      </c>
+      <c r="G18">
+        <v>136.6</v>
+      </c>
+      <c r="H18">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="I18">
+        <v>142.5</v>
+      </c>
+      <c r="J18">
+        <v>146.69999999999999</v>
+      </c>
+      <c r="K18">
+        <v>151</v>
+      </c>
+      <c r="L18">
+        <v>155.1</v>
+      </c>
+      <c r="M18">
+        <v>157.5</v>
+      </c>
+      <c r="N18">
+        <v>159.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>153.30000000000001</v>
+      </c>
+      <c r="E19">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="F19">
+        <v>141.69999999999999</v>
+      </c>
+      <c r="G19">
+        <v>143.1</v>
+      </c>
+      <c r="H19">
+        <v>145.30000000000001</v>
+      </c>
+      <c r="I19">
+        <v>149</v>
+      </c>
+      <c r="J19">
+        <v>153.30000000000001</v>
+      </c>
+      <c r="K19">
+        <v>157.69999999999999</v>
+      </c>
+      <c r="L19">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="M19">
+        <v>164.3</v>
+      </c>
+      <c r="N19">
+        <v>165.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>159.4</v>
+      </c>
+      <c r="E20">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="F20">
+        <v>147.80000000000001</v>
+      </c>
+      <c r="G20">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="H20">
+        <v>151.4</v>
+      </c>
+      <c r="I20">
+        <v>155.1</v>
+      </c>
+      <c r="J20">
+        <v>159.4</v>
+      </c>
+      <c r="K20">
+        <v>163.80000000000001</v>
+      </c>
+      <c r="L20">
+        <v>167.8</v>
+      </c>
+      <c r="M20">
+        <v>170.3</v>
+      </c>
+      <c r="N20">
+        <v>171.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>163.4</v>
+      </c>
+      <c r="E21">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="F21">
+        <v>152</v>
+      </c>
+      <c r="G21">
+        <v>153.4</v>
+      </c>
+      <c r="H21">
+        <v>155.6</v>
+      </c>
+      <c r="I21">
+        <v>159.19999999999999</v>
+      </c>
+      <c r="J21">
+        <v>163.4</v>
+      </c>
+      <c r="K21">
+        <v>167.7</v>
+      </c>
+      <c r="L21">
+        <v>171.6</v>
+      </c>
+      <c r="M21">
+        <v>174.1</v>
+      </c>
+      <c r="N21">
+        <v>175.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>165.5</v>
+      </c>
+      <c r="E22">
+        <v>3.7400000000000003E-2</v>
+      </c>
+      <c r="F22">
+        <v>154.30000000000001</v>
+      </c>
+      <c r="G22">
+        <v>155.6</v>
+      </c>
+      <c r="H22">
+        <v>157.80000000000001</v>
+      </c>
+      <c r="I22">
+        <v>161.4</v>
+      </c>
+      <c r="J22">
+        <v>165.5</v>
+      </c>
+      <c r="K22">
+        <v>169.7</v>
+      </c>
+      <c r="L22">
+        <v>173.6</v>
+      </c>
+      <c r="M22">
+        <v>176</v>
+      </c>
+      <c r="N22">
+        <v>177.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>166.5</v>
+      </c>
+      <c r="E23">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="F23">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="G23">
+        <v>156.69999999999999</v>
+      </c>
+      <c r="H23">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="I23">
+        <v>162.4</v>
+      </c>
+      <c r="J23">
+        <v>166.5</v>
+      </c>
+      <c r="K23">
+        <v>170.7</v>
+      </c>
+      <c r="L23">
+        <v>174.6</v>
+      </c>
+      <c r="M23">
+        <v>176.9</v>
+      </c>
+      <c r="N23">
+        <v>178.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>166.6</v>
+      </c>
+      <c r="E24">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="F24">
+        <v>155.4</v>
+      </c>
+      <c r="G24">
+        <v>156.80000000000001</v>
+      </c>
+      <c r="H24">
+        <v>158.9</v>
+      </c>
+      <c r="I24">
+        <v>162.5</v>
+      </c>
+      <c r="J24">
+        <v>166.6</v>
+      </c>
+      <c r="K24">
+        <v>170.8</v>
+      </c>
+      <c r="L24">
+        <v>174.7</v>
+      </c>
+      <c r="M24">
+        <v>177</v>
+      </c>
+      <c r="N24">
+        <v>178.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>166.8</v>
+      </c>
+      <c r="E25">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="F25">
+        <v>155.6</v>
+      </c>
+      <c r="G25">
+        <v>157</v>
+      </c>
+      <c r="H25">
+        <v>159.1</v>
+      </c>
+      <c r="I25">
+        <v>162.69999999999999</v>
+      </c>
+      <c r="J25">
+        <v>166.8</v>
+      </c>
+      <c r="K25">
+        <v>171</v>
+      </c>
+      <c r="L25">
+        <v>174.9</v>
+      </c>
+      <c r="M25">
+        <v>177.2</v>
+      </c>
+      <c r="N25">
+        <v>178.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C353493-9061-2E46-887D-7324CBFB8386}">
   <dimension ref="A1:F35"/>
   <sheetViews>
@@ -31121,11 +34467,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4643ECC-1455-254C-B38F-4BE8DEA7347B}">
   <dimension ref="A1:D218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Growth reference data and plot function update
</commit_message>
<xml_diff>
--- a/data-raw/maturation.xlsx
+++ b/data-raw/maturation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdukikhia/Documents/R Packages/ageR/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9F0789-BFD6-3A46-8026-3F6BC3452C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157594EF-8484-1945-9A11-0238F1D0B133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="17640" firstSheet="3" activeTab="4" xr2:uid="{1F346313-5E37-0D4E-9152-608513635295}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="Zscores" sheetId="5" r:id="rId8"/>
     <sheet name="Bio Age" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="75">
   <si>
     <t>Player Name</t>
   </si>
@@ -16545,7 +16545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509422DF-31AA-0541-89F7-F5887C8856E2}">
   <dimension ref="A1:N315"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -31531,10 +31531,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B621282F-4F3F-1E46-9D17-20CBB6F27887}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32113,90 +32113,90 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>123</v>
+        <v>180.2</v>
       </c>
       <c r="E14">
-        <v>4.2999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F14">
-        <v>113.4</v>
+        <v>167.8</v>
       </c>
       <c r="G14">
-        <v>114.6</v>
+        <v>169.3</v>
       </c>
       <c r="H14">
-        <v>116.4</v>
+        <v>171.6</v>
       </c>
       <c r="I14">
-        <v>119.5</v>
+        <v>175.6</v>
       </c>
       <c r="J14">
-        <v>123</v>
+        <v>180.2</v>
       </c>
       <c r="K14">
-        <v>126.6</v>
+        <v>184.9</v>
       </c>
       <c r="L14">
-        <v>130</v>
+        <v>189.2</v>
       </c>
       <c r="M14">
-        <v>132</v>
+        <v>191.8</v>
       </c>
       <c r="N14">
-        <v>133.4</v>
+        <v>193.6</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>129</v>
+        <v>180.8</v>
       </c>
       <c r="E15">
-        <v>4.3999999999999997E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F15">
-        <v>118.8</v>
+        <v>168.6</v>
       </c>
       <c r="G15">
-        <v>120</v>
+        <v>170.1</v>
       </c>
       <c r="H15">
-        <v>121.9</v>
+        <v>172.4</v>
       </c>
       <c r="I15">
-        <v>125.2</v>
+        <v>176.3</v>
       </c>
       <c r="J15">
-        <v>129</v>
+        <v>180.8</v>
       </c>
       <c r="K15">
-        <v>132.9</v>
+        <v>185.4</v>
       </c>
       <c r="L15">
-        <v>136.5</v>
+        <v>189.6</v>
       </c>
       <c r="M15">
-        <v>138.69999999999999</v>
+        <v>192.1</v>
       </c>
       <c r="N15">
-        <v>140.1</v>
+        <v>193.8</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -32204,43 +32204,43 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>134.30000000000001</v>
+        <v>123</v>
       </c>
       <c r="E16">
-        <v>4.3999999999999997E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="F16">
-        <v>123.6</v>
+        <v>113.4</v>
       </c>
       <c r="G16">
-        <v>124.9</v>
+        <v>114.6</v>
       </c>
       <c r="H16">
-        <v>126.9</v>
+        <v>116.4</v>
       </c>
       <c r="I16">
-        <v>130.4</v>
+        <v>119.5</v>
       </c>
       <c r="J16">
-        <v>134.30000000000001</v>
+        <v>123</v>
       </c>
       <c r="K16">
-        <v>138.30000000000001</v>
+        <v>126.6</v>
       </c>
       <c r="L16">
-        <v>142.1</v>
+        <v>130</v>
       </c>
       <c r="M16">
-        <v>144.4</v>
+        <v>132</v>
       </c>
       <c r="N16">
-        <v>145.9</v>
+        <v>133.4</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -32248,43 +32248,43 @@
         <v>32</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>139.9</v>
+        <v>129</v>
       </c>
       <c r="E17">
-        <v>4.5999999999999999E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F17">
-        <v>128.30000000000001</v>
+        <v>118.8</v>
       </c>
       <c r="G17">
-        <v>129.69999999999999</v>
+        <v>120</v>
       </c>
       <c r="H17">
-        <v>131.9</v>
+        <v>121.9</v>
       </c>
       <c r="I17">
-        <v>135.6</v>
+        <v>125.2</v>
       </c>
       <c r="J17">
-        <v>139.9</v>
+        <v>129</v>
       </c>
       <c r="K17">
-        <v>144.30000000000001</v>
+        <v>132.9</v>
       </c>
       <c r="L17">
-        <v>148.4</v>
+        <v>136.5</v>
       </c>
       <c r="M17">
-        <v>150.9</v>
+        <v>138.69999999999999</v>
       </c>
       <c r="N17">
-        <v>152.5</v>
+        <v>140.1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -32292,43 +32292,43 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>146.6</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="E18">
-        <v>4.7E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F18">
-        <v>134.19999999999999</v>
+        <v>123.6</v>
       </c>
       <c r="G18">
-        <v>135.69999999999999</v>
+        <v>124.9</v>
       </c>
       <c r="H18">
-        <v>138</v>
+        <v>126.9</v>
       </c>
       <c r="I18">
-        <v>142</v>
+        <v>130.4</v>
       </c>
       <c r="J18">
-        <v>146.6</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="K18">
-        <v>151.30000000000001</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="L18">
-        <v>155.69999999999999</v>
+        <v>142.1</v>
       </c>
       <c r="M18">
-        <v>158.4</v>
+        <v>144.4</v>
       </c>
       <c r="N18">
-        <v>160.1</v>
+        <v>145.9</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -32336,43 +32336,43 @@
         <v>32</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>153.19999999999999</v>
+        <v>139.9</v>
       </c>
       <c r="E19">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F19">
-        <v>140.5</v>
+        <v>128.30000000000001</v>
       </c>
       <c r="G19">
-        <v>142</v>
+        <v>129.69999999999999</v>
       </c>
       <c r="H19">
-        <v>144.4</v>
+        <v>131.9</v>
       </c>
       <c r="I19">
-        <v>148.5</v>
+        <v>135.6</v>
       </c>
       <c r="J19">
-        <v>153.19999999999999</v>
+        <v>139.9</v>
       </c>
       <c r="K19">
-        <v>158</v>
+        <v>144.30000000000001</v>
       </c>
       <c r="L19">
-        <v>162.5</v>
+        <v>148.4</v>
       </c>
       <c r="M19">
-        <v>165.2</v>
+        <v>150.9</v>
       </c>
       <c r="N19">
-        <v>167</v>
+        <v>152.5</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -32380,43 +32380,43 @@
         <v>32</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>158.69999999999999</v>
+        <v>146.6</v>
       </c>
       <c r="E20">
-        <v>4.2999999999999997E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="F20">
-        <v>146.4</v>
+        <v>134.19999999999999</v>
       </c>
       <c r="G20">
-        <v>147.9</v>
+        <v>135.69999999999999</v>
       </c>
       <c r="H20">
-        <v>150.19999999999999</v>
+        <v>138</v>
       </c>
       <c r="I20">
-        <v>154.19999999999999</v>
+        <v>142</v>
       </c>
       <c r="J20">
-        <v>158.69999999999999</v>
+        <v>146.6</v>
       </c>
       <c r="K20">
-        <v>163.4</v>
+        <v>151.30000000000001</v>
       </c>
       <c r="L20">
-        <v>167.7</v>
+        <v>155.69999999999999</v>
       </c>
       <c r="M20">
-        <v>170.3</v>
+        <v>158.4</v>
       </c>
       <c r="N20">
-        <v>172.1</v>
+        <v>160.1</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -32424,43 +32424,43 @@
         <v>32</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>162.4</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="E21">
-        <v>0.04</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="F21">
-        <v>150.6</v>
+        <v>140.5</v>
       </c>
       <c r="G21">
-        <v>152.1</v>
+        <v>142</v>
       </c>
       <c r="H21">
-        <v>154.30000000000001</v>
+        <v>144.4</v>
       </c>
       <c r="I21">
-        <v>158.1</v>
+        <v>148.5</v>
       </c>
       <c r="J21">
-        <v>162.4</v>
+        <v>153.19999999999999</v>
       </c>
       <c r="K21">
-        <v>166.8</v>
+        <v>158</v>
       </c>
       <c r="L21">
-        <v>170.9</v>
+        <v>162.5</v>
       </c>
       <c r="M21">
-        <v>173.4</v>
+        <v>165.2</v>
       </c>
       <c r="N21">
-        <v>175.1</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -32468,43 +32468,43 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>164.7</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="E22">
-        <v>3.7999999999999999E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="F22">
-        <v>153.30000000000001</v>
+        <v>146.4</v>
       </c>
       <c r="G22">
-        <v>154.69999999999999</v>
+        <v>147.9</v>
       </c>
       <c r="H22">
-        <v>156.9</v>
+        <v>150.19999999999999</v>
       </c>
       <c r="I22">
-        <v>160.5</v>
+        <v>154.19999999999999</v>
       </c>
       <c r="J22">
-        <v>164.7</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="K22">
-        <v>169</v>
+        <v>163.4</v>
       </c>
       <c r="L22">
-        <v>172.9</v>
+        <v>167.7</v>
       </c>
       <c r="M22">
-        <v>175.3</v>
+        <v>170.3</v>
       </c>
       <c r="N22">
-        <v>176.9</v>
+        <v>172.1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -32512,43 +32512,43 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>165.8</v>
+        <v>162.4</v>
       </c>
       <c r="E23">
-        <v>3.5999999999999997E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F23">
-        <v>154.9</v>
+        <v>150.6</v>
       </c>
       <c r="G23">
-        <v>156.30000000000001</v>
+        <v>152.1</v>
       </c>
       <c r="H23">
-        <v>158.30000000000001</v>
+        <v>154.30000000000001</v>
       </c>
       <c r="I23">
-        <v>161.80000000000001</v>
+        <v>158.1</v>
       </c>
       <c r="J23">
-        <v>165.8</v>
+        <v>162.4</v>
       </c>
       <c r="K23">
-        <v>169.9</v>
+        <v>166.8</v>
       </c>
       <c r="L23">
-        <v>173.6</v>
+        <v>170.9</v>
       </c>
       <c r="M23">
-        <v>175.9</v>
+        <v>173.4</v>
       </c>
       <c r="N23">
-        <v>177.4</v>
+        <v>175.1</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -32556,43 +32556,43 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>166.2</v>
+        <v>164.7</v>
       </c>
       <c r="E24">
-        <v>3.5999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F24">
-        <v>155.30000000000001</v>
+        <v>153.30000000000001</v>
       </c>
       <c r="G24">
-        <v>156.6</v>
+        <v>154.69999999999999</v>
       </c>
       <c r="H24">
-        <v>158.69999999999999</v>
+        <v>156.9</v>
       </c>
       <c r="I24">
-        <v>162.19999999999999</v>
+        <v>160.5</v>
       </c>
       <c r="J24">
-        <v>166.2</v>
+        <v>164.7</v>
       </c>
       <c r="K24">
-        <v>170.3</v>
+        <v>169</v>
       </c>
       <c r="L24">
-        <v>174</v>
+        <v>172.9</v>
       </c>
       <c r="M24">
-        <v>176.3</v>
+        <v>175.3</v>
       </c>
       <c r="N24">
-        <v>177.8</v>
+        <v>176.9</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -32600,43 +32600,219 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>166.3</v>
+        <v>165.8</v>
       </c>
       <c r="E25">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F25">
+        <v>154.9</v>
+      </c>
+      <c r="G25">
+        <v>156.30000000000001</v>
+      </c>
+      <c r="H25">
+        <v>158.30000000000001</v>
+      </c>
+      <c r="I25">
+        <v>161.80000000000001</v>
+      </c>
+      <c r="J25">
+        <v>165.8</v>
+      </c>
+      <c r="K25">
+        <v>169.9</v>
+      </c>
+      <c r="L25">
+        <v>173.6</v>
+      </c>
+      <c r="M25">
+        <v>175.9</v>
+      </c>
+      <c r="N25">
+        <v>177.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>166.2</v>
+      </c>
+      <c r="E26">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F26">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="G26">
+        <v>156.6</v>
+      </c>
+      <c r="H26">
+        <v>158.69999999999999</v>
+      </c>
+      <c r="I26">
+        <v>162.19999999999999</v>
+      </c>
+      <c r="J26">
+        <v>166.2</v>
+      </c>
+      <c r="K26">
+        <v>170.3</v>
+      </c>
+      <c r="L26">
+        <v>174</v>
+      </c>
+      <c r="M26">
+        <v>176.3</v>
+      </c>
+      <c r="N26">
+        <v>177.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>166.3</v>
+      </c>
+      <c r="E27">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F27">
         <v>155.4</v>
       </c>
-      <c r="G25">
+      <c r="G27">
         <v>156.69999999999999</v>
       </c>
-      <c r="H25">
+      <c r="H27">
         <v>158.80000000000001</v>
       </c>
-      <c r="I25">
+      <c r="I27">
         <v>162.30000000000001</v>
       </c>
-      <c r="J25">
+      <c r="J27">
         <v>166.3</v>
       </c>
-      <c r="K25">
+      <c r="K27">
         <v>170.4</v>
       </c>
-      <c r="L25">
+      <c r="L27">
         <v>174.2</v>
       </c>
-      <c r="M25">
+      <c r="M27">
         <v>176.4</v>
       </c>
-      <c r="N25">
+      <c r="N27">
         <v>177.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>166.4</v>
+      </c>
+      <c r="E28">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F28">
+        <v>155.5</v>
+      </c>
+      <c r="G28">
+        <v>156.80000000000001</v>
+      </c>
+      <c r="H28">
+        <v>158.9</v>
+      </c>
+      <c r="I28">
+        <v>162.4</v>
+      </c>
+      <c r="J28">
+        <v>166.4</v>
+      </c>
+      <c r="K28">
+        <v>170.5</v>
+      </c>
+      <c r="L28">
+        <v>174.3</v>
+      </c>
+      <c r="M28">
+        <v>176.6</v>
+      </c>
+      <c r="N28">
+        <v>178.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>166.5</v>
+      </c>
+      <c r="E29">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F29">
+        <v>155.6</v>
+      </c>
+      <c r="G29">
+        <v>156.9</v>
+      </c>
+      <c r="H29">
+        <v>159</v>
+      </c>
+      <c r="I29">
+        <v>162.5</v>
+      </c>
+      <c r="J29">
+        <v>166.5</v>
+      </c>
+      <c r="K29">
+        <v>170.6</v>
+      </c>
+      <c r="L29">
+        <v>174.4</v>
+      </c>
+      <c r="M29">
+        <v>176.7</v>
+      </c>
+      <c r="N29">
+        <v>178.2</v>
       </c>
     </row>
   </sheetData>
@@ -32646,10 +32822,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEEADE3-FC3F-9840-9458-6D9E58369C21}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33228,46 +33404,46 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>123.8</v>
+        <v>181</v>
       </c>
       <c r="E14">
-        <v>4.2299999999999997E-2</v>
+        <v>3.6299999999999999E-2</v>
       </c>
       <c r="F14">
-        <v>114.3</v>
+        <v>169.1</v>
       </c>
       <c r="G14">
-        <v>115.5</v>
+        <v>170.5</v>
       </c>
       <c r="H14">
-        <v>117.3</v>
+        <v>172.8</v>
       </c>
       <c r="I14">
-        <v>120.3</v>
+        <v>176.6</v>
       </c>
       <c r="J14">
-        <v>123.8</v>
+        <v>181</v>
       </c>
       <c r="K14">
-        <v>127.4</v>
+        <v>185.5</v>
       </c>
       <c r="L14">
-        <v>130.69999999999999</v>
+        <v>189.6</v>
       </c>
       <c r="M14">
-        <v>132.69999999999999</v>
+        <v>192.1</v>
       </c>
       <c r="N14">
-        <v>134.1</v>
+        <v>193.8</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -33275,43 +33451,43 @@
         <v>32</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>129.80000000000001</v>
+        <v>123.8</v>
       </c>
       <c r="E15">
-        <v>4.2900000000000001E-2</v>
+        <v>4.2299999999999997E-2</v>
       </c>
       <c r="F15">
-        <v>119.7</v>
+        <v>114.3</v>
       </c>
       <c r="G15">
-        <v>121</v>
+        <v>115.5</v>
       </c>
       <c r="H15">
-        <v>122.9</v>
+        <v>117.3</v>
       </c>
       <c r="I15">
-        <v>126.1</v>
+        <v>120.3</v>
       </c>
       <c r="J15">
-        <v>129.80000000000001</v>
+        <v>123.8</v>
       </c>
       <c r="K15">
-        <v>133.6</v>
+        <v>127.4</v>
       </c>
       <c r="L15">
-        <v>137.1</v>
+        <v>130.69999999999999</v>
       </c>
       <c r="M15">
-        <v>139.30000000000001</v>
+        <v>132.69999999999999</v>
       </c>
       <c r="N15">
-        <v>140.69999999999999</v>
+        <v>134.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -33319,43 +33495,43 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16">
-        <v>135</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="E16">
-        <v>4.3299999999999998E-2</v>
+        <v>4.2900000000000001E-2</v>
       </c>
       <c r="F16">
-        <v>124.4</v>
+        <v>119.7</v>
       </c>
       <c r="G16">
-        <v>125.7</v>
+        <v>121</v>
       </c>
       <c r="H16">
-        <v>127.7</v>
+        <v>122.9</v>
       </c>
       <c r="I16">
-        <v>131.1</v>
+        <v>126.1</v>
       </c>
       <c r="J16">
-        <v>135</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="K16">
-        <v>139</v>
+        <v>133.6</v>
       </c>
       <c r="L16">
-        <v>142.69999999999999</v>
+        <v>137.1</v>
       </c>
       <c r="M16">
-        <v>145</v>
+        <v>139.30000000000001</v>
       </c>
       <c r="N16">
-        <v>146.5</v>
+        <v>140.69999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -33363,43 +33539,43 @@
         <v>32</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>140.5</v>
+        <v>135</v>
       </c>
       <c r="E17">
-        <v>4.3499999999999997E-2</v>
+        <v>4.3299999999999998E-2</v>
       </c>
       <c r="F17">
-        <v>129.5</v>
+        <v>124.4</v>
       </c>
       <c r="G17">
-        <v>130.80000000000001</v>
+        <v>125.7</v>
       </c>
       <c r="H17">
-        <v>132.9</v>
+        <v>127.7</v>
       </c>
       <c r="I17">
-        <v>136.4</v>
+        <v>131.1</v>
       </c>
       <c r="J17">
-        <v>140.5</v>
+        <v>135</v>
       </c>
       <c r="K17">
-        <v>144.69999999999999</v>
+        <v>139</v>
       </c>
       <c r="L17">
-        <v>148.6</v>
+        <v>142.69999999999999</v>
       </c>
       <c r="M17">
-        <v>150.9</v>
+        <v>145</v>
       </c>
       <c r="N17">
-        <v>152.5</v>
+        <v>146.5</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -33407,43 +33583,43 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18">
-        <v>146.69999999999999</v>
+        <v>140.5</v>
       </c>
       <c r="E18">
-        <v>4.3200000000000002E-2</v>
+        <v>4.3499999999999997E-2</v>
       </c>
       <c r="F18">
-        <v>135.30000000000001</v>
+        <v>129.5</v>
       </c>
       <c r="G18">
-        <v>136.6</v>
+        <v>130.80000000000001</v>
       </c>
       <c r="H18">
-        <v>138.80000000000001</v>
+        <v>132.9</v>
       </c>
       <c r="I18">
-        <v>142.5</v>
+        <v>136.4</v>
       </c>
       <c r="J18">
-        <v>146.69999999999999</v>
+        <v>140.5</v>
       </c>
       <c r="K18">
-        <v>151</v>
+        <v>144.69999999999999</v>
       </c>
       <c r="L18">
-        <v>155.1</v>
+        <v>148.6</v>
       </c>
       <c r="M18">
-        <v>157.5</v>
+        <v>150.9</v>
       </c>
       <c r="N18">
-        <v>159.1</v>
+        <v>152.5</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -33451,43 +33627,43 @@
         <v>32</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>153.30000000000001</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="E19">
-        <v>4.2000000000000003E-2</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="F19">
-        <v>141.69999999999999</v>
+        <v>135.30000000000001</v>
       </c>
       <c r="G19">
-        <v>143.1</v>
+        <v>136.6</v>
       </c>
       <c r="H19">
-        <v>145.30000000000001</v>
+        <v>138.80000000000001</v>
       </c>
       <c r="I19">
-        <v>149</v>
+        <v>142.5</v>
       </c>
       <c r="J19">
-        <v>153.30000000000001</v>
+        <v>146.69999999999999</v>
       </c>
       <c r="K19">
-        <v>157.69999999999999</v>
+        <v>151</v>
       </c>
       <c r="L19">
-        <v>161.80000000000001</v>
+        <v>155.1</v>
       </c>
       <c r="M19">
-        <v>164.3</v>
+        <v>157.5</v>
       </c>
       <c r="N19">
-        <v>165.9</v>
+        <v>159.1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -33495,43 +33671,43 @@
         <v>32</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20">
-        <v>159.4</v>
+        <v>153.30000000000001</v>
       </c>
       <c r="E20">
-        <v>4.0099999999999997E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="F20">
-        <v>147.80000000000001</v>
+        <v>141.69999999999999</v>
       </c>
       <c r="G20">
-        <v>149.19999999999999</v>
+        <v>143.1</v>
       </c>
       <c r="H20">
-        <v>151.4</v>
+        <v>145.30000000000001</v>
       </c>
       <c r="I20">
-        <v>155.1</v>
+        <v>149</v>
       </c>
       <c r="J20">
-        <v>159.4</v>
+        <v>153.30000000000001</v>
       </c>
       <c r="K20">
-        <v>163.80000000000001</v>
+        <v>157.69999999999999</v>
       </c>
       <c r="L20">
-        <v>167.8</v>
+        <v>161.80000000000001</v>
       </c>
       <c r="M20">
-        <v>170.3</v>
+        <v>164.3</v>
       </c>
       <c r="N20">
-        <v>171.9</v>
+        <v>165.9</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -33539,43 +33715,43 @@
         <v>32</v>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>163.4</v>
+        <v>159.4</v>
       </c>
       <c r="E21">
-        <v>3.8399999999999997E-2</v>
+        <v>4.0099999999999997E-2</v>
       </c>
       <c r="F21">
-        <v>152</v>
+        <v>147.80000000000001</v>
       </c>
       <c r="G21">
-        <v>153.4</v>
+        <v>149.19999999999999</v>
       </c>
       <c r="H21">
-        <v>155.6</v>
+        <v>151.4</v>
       </c>
       <c r="I21">
-        <v>159.19999999999999</v>
+        <v>155.1</v>
       </c>
       <c r="J21">
-        <v>163.4</v>
+        <v>159.4</v>
       </c>
       <c r="K21">
-        <v>167.7</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="L21">
-        <v>171.6</v>
+        <v>167.8</v>
       </c>
       <c r="M21">
-        <v>174.1</v>
+        <v>170.3</v>
       </c>
       <c r="N21">
-        <v>175.6</v>
+        <v>171.9</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -33583,43 +33759,43 @@
         <v>32</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22">
-        <v>165.5</v>
+        <v>163.4</v>
       </c>
       <c r="E22">
-        <v>3.7400000000000003E-2</v>
+        <v>3.8399999999999997E-2</v>
       </c>
       <c r="F22">
-        <v>154.30000000000001</v>
+        <v>152</v>
       </c>
       <c r="G22">
+        <v>153.4</v>
+      </c>
+      <c r="H22">
         <v>155.6</v>
       </c>
-      <c r="H22">
-        <v>157.80000000000001</v>
-      </c>
       <c r="I22">
-        <v>161.4</v>
+        <v>159.19999999999999</v>
       </c>
       <c r="J22">
-        <v>165.5</v>
+        <v>163.4</v>
       </c>
       <c r="K22">
-        <v>169.7</v>
+        <v>167.7</v>
       </c>
       <c r="L22">
-        <v>173.6</v>
+        <v>171.6</v>
       </c>
       <c r="M22">
-        <v>176</v>
+        <v>174.1</v>
       </c>
       <c r="N22">
-        <v>177.6</v>
+        <v>175.6</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -33627,43 +33803,43 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>166.5</v>
+        <v>165.5</v>
       </c>
       <c r="E23">
-        <v>3.6999999999999998E-2</v>
+        <v>3.7400000000000003E-2</v>
       </c>
       <c r="F23">
-        <v>155.30000000000001</v>
+        <v>154.30000000000001</v>
       </c>
       <c r="G23">
-        <v>156.69999999999999</v>
+        <v>155.6</v>
       </c>
       <c r="H23">
-        <v>158.80000000000001</v>
+        <v>157.80000000000001</v>
       </c>
       <c r="I23">
-        <v>162.4</v>
+        <v>161.4</v>
       </c>
       <c r="J23">
-        <v>166.5</v>
+        <v>165.5</v>
       </c>
       <c r="K23">
-        <v>170.7</v>
+        <v>169.7</v>
       </c>
       <c r="L23">
-        <v>174.6</v>
+        <v>173.6</v>
       </c>
       <c r="M23">
-        <v>176.9</v>
+        <v>176</v>
       </c>
       <c r="N23">
-        <v>178.5</v>
+        <v>177.6</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -33671,43 +33847,43 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24">
-        <v>166.6</v>
+        <v>166.5</v>
       </c>
       <c r="E24">
-        <v>3.6900000000000002E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="F24">
-        <v>155.4</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="G24">
-        <v>156.80000000000001</v>
+        <v>156.69999999999999</v>
       </c>
       <c r="H24">
-        <v>158.9</v>
+        <v>158.80000000000001</v>
       </c>
       <c r="I24">
-        <v>162.5</v>
+        <v>162.4</v>
       </c>
       <c r="J24">
-        <v>166.6</v>
+        <v>166.5</v>
       </c>
       <c r="K24">
-        <v>170.8</v>
+        <v>170.7</v>
       </c>
       <c r="L24">
-        <v>174.7</v>
+        <v>174.6</v>
       </c>
       <c r="M24">
-        <v>177</v>
+        <v>176.9</v>
       </c>
       <c r="N24">
-        <v>178.6</v>
+        <v>178.5</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
@@ -33715,43 +33891,131 @@
         <v>32</v>
       </c>
       <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>166.6</v>
+      </c>
+      <c r="E25">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="F25">
+        <v>155.4</v>
+      </c>
+      <c r="G25">
+        <v>156.80000000000001</v>
+      </c>
+      <c r="H25">
+        <v>158.9</v>
+      </c>
+      <c r="I25">
+        <v>162.5</v>
+      </c>
+      <c r="J25">
+        <v>166.6</v>
+      </c>
+      <c r="K25">
+        <v>170.8</v>
+      </c>
+      <c r="L25">
+        <v>174.7</v>
+      </c>
+      <c r="M25">
+        <v>177</v>
+      </c>
+      <c r="N25">
+        <v>178.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26">
         <v>18</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
         <v>166.8</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>3.6799999999999999E-2</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>155.6</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>157</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>159.1</v>
       </c>
-      <c r="I25">
+      <c r="I26">
         <v>162.69999999999999</v>
       </c>
-      <c r="J25">
+      <c r="J26">
         <v>166.8</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <v>171</v>
       </c>
-      <c r="L25">
+      <c r="L26">
         <v>174.9</v>
       </c>
-      <c r="M25">
+      <c r="M26">
         <v>177.2</v>
       </c>
-      <c r="N25">
+      <c r="N26">
         <v>178.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>167.2</v>
+      </c>
+      <c r="E27">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="F27">
+        <v>156.1</v>
+      </c>
+      <c r="G27">
+        <v>157.4</v>
+      </c>
+      <c r="H27">
+        <v>159.5</v>
+      </c>
+      <c r="I27">
+        <v>163.1</v>
+      </c>
+      <c r="J27">
+        <v>167.2</v>
+      </c>
+      <c r="K27">
+        <v>171.4</v>
+      </c>
+      <c r="L27">
+        <v>175.2</v>
+      </c>
+      <c r="M27">
+        <v>177.6</v>
+      </c>
+      <c r="N27">
+        <v>179.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>